<commit_message>
Adding foram metadata (new project)
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/unige/desalt/metadata.xlsx
+++ b/metadata/excel/projects/unige/desalt/metadata.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="900" yWindow="940" windowWidth="26720" windowHeight="20520" tabRatio="500"/>
+    <workbookView xWindow="6140" yWindow="1980" windowWidth="44080" windowHeight="25000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="micans_v6_ex1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="400">
   <si>
     <t>Country</t>
   </si>
@@ -1172,13 +1172,169 @@
   <si>
     <t>Israel</t>
   </si>
+  <si>
+    <t>Near Dorad power station</t>
+  </si>
+  <si>
+    <t>Nearer Dorad power station</t>
+  </si>
+  <si>
+    <t>Near Ashkelon</t>
+  </si>
+  <si>
+    <t>Near Palmahim</t>
+  </si>
+  <si>
+    <t>Palmahim coast</t>
+  </si>
+  <si>
+    <t>Nearer Orot Rabin power plant</t>
+  </si>
+  <si>
+    <t>Near Gedor Sea Reserve</t>
+  </si>
+  <si>
+    <t>Near Orot Rabin power plant</t>
+  </si>
+  <si>
+    <t>8511bc3198210a1e0cd5e8c9b637324a</t>
+  </si>
+  <si>
+    <t>047a8ee108bb27f49ed528594bf6d0a8</t>
+  </si>
+  <si>
+    <t>56c7d5330fba5ed7b14932b047c03596</t>
+  </si>
+  <si>
+    <t>d35cdb5a4f9cfe18797f424464de12f5</t>
+  </si>
+  <si>
+    <t>7f6787ea3e324f2e90e0d770cabfa0f0</t>
+  </si>
+  <si>
+    <t>e2d59ea5d7bf5d7cf6f58874d4c2ed08</t>
+  </si>
+  <si>
+    <t>2d4a561351f524a554b8d0425e18a19e</t>
+  </si>
+  <si>
+    <t>5fb1f61812bae135a4fe2f2d6319f8fa</t>
+  </si>
+  <si>
+    <t>50a4524c32be2c5429e4bca8ea093fd6</t>
+  </si>
+  <si>
+    <t>a2c98d76f0641ae7bab0bbe61285cb3a</t>
+  </si>
+  <si>
+    <t>e48a33d9956aad90abfc6c37cd675fc5</t>
+  </si>
+  <si>
+    <t>7a15d0fbbbc0d6120d2f5c8486ee7d4d</t>
+  </si>
+  <si>
+    <t>732160d5f644d5226ef0c6c71493f6b9</t>
+  </si>
+  <si>
+    <t>9f89a5b7d5ec2922771ff01bf1de6cec</t>
+  </si>
+  <si>
+    <t>3ef31ce9f4bff44432e59884887198b2</t>
+  </si>
+  <si>
+    <t>95bc43f970fe906b2c532f603c74a6f3</t>
+  </si>
+  <si>
+    <t>36d55e55b1c607b2100ac4e82558c1d6</t>
+  </si>
+  <si>
+    <t>99179dea456715da3471dfd5c18e4e64</t>
+  </si>
+  <si>
+    <t>207b88113a59aadcb456c2087df15378</t>
+  </si>
+  <si>
+    <t>ee6f6e1e3131938c3959b22a81b600d2</t>
+  </si>
+  <si>
+    <t>cdb5f0be86fbaeea45931f2731ec9fca</t>
+  </si>
+  <si>
+    <t>419958f5b6e95a51309d3e185772e21f</t>
+  </si>
+  <si>
+    <t>7c6d3a88317f117fef419df3b9460d31</t>
+  </si>
+  <si>
+    <t>c3bce9493fab9d4c0c8a6e81b245d466</t>
+  </si>
+  <si>
+    <t>2faf7896d2416d9b436196c87cc0a6ef</t>
+  </si>
+  <si>
+    <t>1e003039892117bc108c6a3f0bcfcb8b</t>
+  </si>
+  <si>
+    <t>b0de3d53105638d85bf4441df22acfde</t>
+  </si>
+  <si>
+    <t>f3eb5028f0d5a53423826659230e1c1f</t>
+  </si>
+  <si>
+    <t>01d37197c23df58b187bd60efc1e0b1f</t>
+  </si>
+  <si>
+    <t>f63ac6429a96c33dac268d77030ce61a</t>
+  </si>
+  <si>
+    <t>6d4fc385c360842ce1ab1a89f1ff7af2</t>
+  </si>
+  <si>
+    <t>3761688d44aafb378599efa70af2c956</t>
+  </si>
+  <si>
+    <t>c7666135294db2faa36ce0ad993f00ea</t>
+  </si>
+  <si>
+    <t>8975ec171784c3f20cc69b4dd51d4542</t>
+  </si>
+  <si>
+    <t>a5e01256600a89d6da74c1585ef2d092</t>
+  </si>
+  <si>
+    <t>7b146d2594c149ed1c5ee5005d68e56c</t>
+  </si>
+  <si>
+    <t>b6e05d1fe7c2921ea4dcb0bf3006c7ee</t>
+  </si>
+  <si>
+    <t>98952afae1ab47969c6b6e0017d53014</t>
+  </si>
+  <si>
+    <t>39b68847b8bd848fed08748f5cbca5c5</t>
+  </si>
+  <si>
+    <t>497d64cc61dd06a69816e123ba621599</t>
+  </si>
+  <si>
+    <t>d4ddf09f5ee7c7d8fb0f3d4af1823e3f</t>
+  </si>
+  <si>
+    <t>3dbbe8445aed5d210175052b9c1672b3</t>
+  </si>
+  <si>
+    <t>9c720889c1555b1ce4410c59cf3ab5c4</t>
+  </si>
+  <si>
+    <t>450667f82bc789cb597fcd7cdbc00e23</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -1428,7 +1584,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="293">
+  <cellStyleXfs count="296">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1722,8 +1878,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1792,18 +1951,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1814,7 +1973,7 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1857,15 +2016,31 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="291" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="291"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="293">
+  <cellStyles count="296">
     <cellStyle name="Excel Built-in Normal" xfId="267"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2023,6 +2198,9 @@
     <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2529,10 +2707,10 @@
   </sheetPr>
   <dimension ref="A1:CB51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="BM25" sqref="BM25"/>
+      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2595,14 +2773,15 @@
     <col min="60" max="61" width="15.5" customWidth="1"/>
     <col min="62" max="62" width="13.6640625" style="11" customWidth="1"/>
     <col min="63" max="63" width="13.1640625" style="11" customWidth="1"/>
-    <col min="64" max="64" width="12.5" style="16" customWidth="1"/>
-    <col min="65" max="65" width="26" style="16" customWidth="1"/>
+    <col min="64" max="64" width="13.1640625" style="68" customWidth="1"/>
+    <col min="65" max="65" width="28" style="16" customWidth="1"/>
     <col min="66" max="66" width="31.33203125" style="16" customWidth="1"/>
     <col min="67" max="67" width="9" customWidth="1"/>
     <col min="68" max="68" width="16.5" customWidth="1"/>
     <col min="69" max="69" width="16" customWidth="1"/>
     <col min="70" max="70" width="9.5" customWidth="1"/>
-    <col min="71" max="72" width="11" style="22" customWidth="1"/>
+    <col min="71" max="71" width="11" style="22" customWidth="1"/>
+    <col min="72" max="72" width="11" style="72" customWidth="1"/>
     <col min="73" max="73" width="11.6640625" style="22" customWidth="1"/>
     <col min="74" max="74" width="14.33203125" style="22" customWidth="1"/>
     <col min="75" max="75" width="12.6640625" style="22" customWidth="1"/>
@@ -2662,29 +2841,29 @@
       <c r="AY1" s="3"/>
       <c r="AZ1" s="3"/>
       <c r="BA1" s="10"/>
-      <c r="BC1" s="65" t="s">
+      <c r="BC1" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="BD1" s="65"/>
-      <c r="BE1" s="65"/>
-      <c r="BF1" s="65"/>
-      <c r="BH1" s="65" t="s">
+      <c r="BD1" s="73"/>
+      <c r="BE1" s="73"/>
+      <c r="BF1" s="73"/>
+      <c r="BH1" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="BI1" s="65"/>
-      <c r="BJ1" s="65"/>
-      <c r="BK1" s="65"/>
-      <c r="BL1" s="65"/>
-      <c r="BM1" s="65"/>
-      <c r="BN1" s="65"/>
-      <c r="BP1" s="65" t="s">
+      <c r="BI1" s="73"/>
+      <c r="BJ1" s="73"/>
+      <c r="BK1" s="73"/>
+      <c r="BL1" s="73"/>
+      <c r="BM1" s="73"/>
+      <c r="BN1" s="73"/>
+      <c r="BP1" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="BQ1" s="65"/>
+      <c r="BQ1" s="73"/>
       <c r="BS1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="BT1" s="8"/>
+      <c r="BT1" s="69"/>
       <c r="BU1" s="21"/>
       <c r="BV1" s="21"/>
       <c r="BW1" s="21"/>
@@ -2913,7 +3092,7 @@
     </row>
     <row r="3" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
-        <f>COUNTIF(D3,"&lt;&gt;"&amp;"")+COUNTIF(BN3,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" ref="A3:A29" si="0">COUNTIF(D3,"&lt;&gt;"&amp;"")+COUNTIF(BN3,"&lt;&gt;"&amp;"")</f>
         <v>1</v>
       </c>
       <c r="B3" s="23">
@@ -2949,10 +3128,18 @@
       <c r="N3" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O3" s="37"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="19"/>
+      <c r="O3" s="37">
+        <v>275162</v>
+      </c>
+      <c r="P3" s="40">
+        <v>275162</v>
+      </c>
+      <c r="Q3" s="54" t="s">
+        <v>356</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>378</v>
+      </c>
       <c r="S3" t="s">
         <v>49</v>
       </c>
@@ -3041,32 +3228,38 @@
         <v>76</v>
       </c>
       <c r="AZ3">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA3">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC3" s="57"/>
       <c r="BD3" s="57"/>
       <c r="BE3" s="57"/>
       <c r="BF3" s="57"/>
-      <c r="BH3" s="66">
+      <c r="BH3" s="65">
         <v>41226</v>
       </c>
-      <c r="BI3" s="67" t="s">
+      <c r="BI3" s="66" t="s">
         <v>335</v>
       </c>
-      <c r="BJ3" s="25"/>
-      <c r="BK3" s="25"/>
-      <c r="BL3" t="s">
+      <c r="BJ3" s="67">
+        <v>31.63212</v>
+      </c>
+      <c r="BK3" s="67">
+        <v>34.5167</v>
+      </c>
+      <c r="BL3" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM3"/>
+      <c r="BM3" t="s">
+        <v>349</v>
+      </c>
       <c r="BN3" s="25"/>
       <c r="BS3">
         <v>1.5</v>
       </c>
-      <c r="BT3" t="s">
+      <c r="BT3" s="42" t="s">
         <v>345</v>
       </c>
       <c r="BU3"/>
@@ -3079,7 +3272,7 @@
     </row>
     <row r="4" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
-        <f>COUNTIF(D4,"&lt;&gt;"&amp;"")+COUNTIF(BN4,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B4" s="23">
@@ -3115,8 +3308,12 @@
       <c r="N4" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O4" s="37"/>
-      <c r="P4" s="40"/>
+      <c r="O4" s="37">
+        <v>0</v>
+      </c>
+      <c r="P4" s="40">
+        <v>0</v>
+      </c>
       <c r="Q4" s="54"/>
       <c r="R4" s="19"/>
       <c r="S4" t="s">
@@ -3207,32 +3404,38 @@
         <v>76</v>
       </c>
       <c r="AZ4">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA4">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC4" s="57"/>
       <c r="BD4" s="57"/>
       <c r="BE4" s="57"/>
       <c r="BF4" s="57"/>
-      <c r="BH4" s="66">
+      <c r="BH4" s="65">
         <v>41226</v>
       </c>
-      <c r="BI4" s="67" t="s">
+      <c r="BI4" s="66" t="s">
         <v>335</v>
       </c>
-      <c r="BJ4" s="25"/>
-      <c r="BK4" s="25"/>
-      <c r="BL4" t="s">
+      <c r="BJ4" s="67">
+        <v>31.63212</v>
+      </c>
+      <c r="BK4" s="67">
+        <v>34.5167</v>
+      </c>
+      <c r="BL4" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM4"/>
+      <c r="BM4" t="s">
+        <v>349</v>
+      </c>
       <c r="BN4" s="25"/>
       <c r="BS4">
         <v>1.5</v>
       </c>
-      <c r="BT4" t="s">
+      <c r="BT4" s="42" t="s">
         <v>345</v>
       </c>
       <c r="BU4"/>
@@ -3245,7 +3448,7 @@
     </row>
     <row r="5" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
-        <f>COUNTIF(D5,"&lt;&gt;"&amp;"")+COUNTIF(BN5,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B5" s="23">
@@ -3281,10 +3484,18 @@
       <c r="N5" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O5" s="37"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="24"/>
+      <c r="O5" s="37">
+        <v>367728</v>
+      </c>
+      <c r="P5" s="40">
+        <v>367728</v>
+      </c>
+      <c r="Q5" s="54" t="s">
+        <v>357</v>
+      </c>
+      <c r="R5" s="24" t="s">
+        <v>379</v>
+      </c>
       <c r="S5" t="s">
         <v>49</v>
       </c>
@@ -3373,32 +3584,38 @@
         <v>76</v>
       </c>
       <c r="AZ5">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA5">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC5" s="57"/>
       <c r="BD5" s="57"/>
       <c r="BE5" s="57"/>
       <c r="BF5" s="57"/>
-      <c r="BH5" s="66">
+      <c r="BH5" s="65">
         <v>41226</v>
       </c>
-      <c r="BI5" s="67" t="s">
+      <c r="BI5" s="66" t="s">
         <v>335</v>
       </c>
-      <c r="BJ5" s="25"/>
-      <c r="BK5" s="25"/>
-      <c r="BL5" t="s">
+      <c r="BJ5" s="67">
+        <v>31.63212</v>
+      </c>
+      <c r="BK5" s="67">
+        <v>34.5167</v>
+      </c>
+      <c r="BL5" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM5"/>
+      <c r="BM5" t="s">
+        <v>349</v>
+      </c>
       <c r="BN5" s="25"/>
       <c r="BS5">
         <v>1.5</v>
       </c>
-      <c r="BT5" t="s">
+      <c r="BT5" s="42" t="s">
         <v>345</v>
       </c>
       <c r="BU5"/>
@@ -3411,7 +3628,7 @@
     </row>
     <row r="6" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
-        <f>COUNTIF(D6,"&lt;&gt;"&amp;"")+COUNTIF(BN6,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B6" s="23">
@@ -3447,10 +3664,18 @@
       <c r="N6" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O6" s="37"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="19"/>
+      <c r="O6" s="37">
+        <v>292281</v>
+      </c>
+      <c r="P6" s="40">
+        <v>292281</v>
+      </c>
+      <c r="Q6" s="55" t="s">
+        <v>358</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>380</v>
+      </c>
       <c r="S6" t="s">
         <v>49</v>
       </c>
@@ -3539,32 +3764,38 @@
         <v>76</v>
       </c>
       <c r="AZ6">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA6">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC6" s="57"/>
       <c r="BD6" s="57"/>
       <c r="BE6" s="57"/>
       <c r="BF6" s="57"/>
-      <c r="BH6" s="66">
+      <c r="BH6" s="65">
         <v>41226</v>
       </c>
-      <c r="BI6" s="67" t="s">
+      <c r="BI6" s="66" t="s">
         <v>336</v>
       </c>
-      <c r="BJ6" s="25"/>
-      <c r="BK6" s="25"/>
-      <c r="BL6" t="s">
+      <c r="BJ6" s="67">
+        <v>31.6341</v>
+      </c>
+      <c r="BK6" s="67">
+        <v>34.51144</v>
+      </c>
+      <c r="BL6" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM6"/>
+      <c r="BM6" t="s">
+        <v>348</v>
+      </c>
       <c r="BN6" s="25"/>
       <c r="BS6">
         <v>10</v>
       </c>
-      <c r="BT6" s="68" t="s">
+      <c r="BT6" s="70" t="s">
         <v>346</v>
       </c>
       <c r="BU6"/>
@@ -3577,7 +3808,7 @@
     </row>
     <row r="7" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
-        <f>COUNTIF(D7,"&lt;&gt;"&amp;"")+COUNTIF(BN7,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B7" s="23">
@@ -3613,10 +3844,18 @@
       <c r="N7" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O7" s="37"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="19"/>
+      <c r="O7" s="37">
+        <v>242696</v>
+      </c>
+      <c r="P7" s="40">
+        <v>242696</v>
+      </c>
+      <c r="Q7" s="54" t="s">
+        <v>359</v>
+      </c>
+      <c r="R7" s="19" t="s">
+        <v>381</v>
+      </c>
       <c r="S7" t="s">
         <v>49</v>
       </c>
@@ -3705,32 +3944,38 @@
         <v>76</v>
       </c>
       <c r="AZ7">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA7">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC7" s="57"/>
       <c r="BD7" s="57"/>
       <c r="BE7" s="57"/>
       <c r="BF7" s="57"/>
-      <c r="BH7" s="66">
+      <c r="BH7" s="65">
         <v>41226</v>
       </c>
-      <c r="BI7" s="67" t="s">
+      <c r="BI7" s="66" t="s">
         <v>336</v>
       </c>
-      <c r="BJ7" s="25"/>
-      <c r="BK7" s="25"/>
-      <c r="BL7" t="s">
+      <c r="BJ7" s="67">
+        <v>31.6341</v>
+      </c>
+      <c r="BK7" s="67">
+        <v>34.51144</v>
+      </c>
+      <c r="BL7" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM7"/>
+      <c r="BM7" t="s">
+        <v>348</v>
+      </c>
       <c r="BN7" s="25"/>
       <c r="BS7">
         <v>10</v>
       </c>
-      <c r="BT7" s="69" t="s">
+      <c r="BT7" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU7"/>
@@ -3743,7 +3988,7 @@
     </row>
     <row r="8" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
-        <f>COUNTIF(D8,"&lt;&gt;"&amp;"")+COUNTIF(BN8,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B8" s="23">
@@ -3779,10 +4024,18 @@
       <c r="N8" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O8" s="37"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="24"/>
+      <c r="O8" s="37">
+        <v>282664</v>
+      </c>
+      <c r="P8" s="40">
+        <v>282664</v>
+      </c>
+      <c r="Q8" s="54" t="s">
+        <v>360</v>
+      </c>
+      <c r="R8" s="24" t="s">
+        <v>382</v>
+      </c>
       <c r="S8" t="s">
         <v>49</v>
       </c>
@@ -3871,32 +4124,38 @@
         <v>76</v>
       </c>
       <c r="AZ8">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA8">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC8" s="57"/>
       <c r="BD8" s="57"/>
       <c r="BE8" s="57"/>
       <c r="BF8" s="57"/>
-      <c r="BH8" s="66">
+      <c r="BH8" s="65">
         <v>41226</v>
       </c>
-      <c r="BI8" s="67" t="s">
+      <c r="BI8" s="66" t="s">
         <v>336</v>
       </c>
-      <c r="BJ8" s="25"/>
-      <c r="BK8" s="25"/>
-      <c r="BL8" t="s">
+      <c r="BJ8" s="67">
+        <v>31.6341</v>
+      </c>
+      <c r="BK8" s="67">
+        <v>34.51144</v>
+      </c>
+      <c r="BL8" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM8"/>
+      <c r="BM8" t="s">
+        <v>348</v>
+      </c>
       <c r="BN8" s="25"/>
       <c r="BS8">
         <v>10</v>
       </c>
-      <c r="BT8" s="69" t="s">
+      <c r="BT8" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU8"/>
@@ -3909,7 +4168,7 @@
     </row>
     <row r="9" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
-        <f>COUNTIF(D9,"&lt;&gt;"&amp;"")+COUNTIF(BN9,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B9" s="23">
@@ -3945,10 +4204,18 @@
       <c r="N9" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O9" s="37"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="19"/>
+      <c r="O9" s="37">
+        <v>233579</v>
+      </c>
+      <c r="P9" s="40">
+        <v>233579</v>
+      </c>
+      <c r="Q9" s="54" t="s">
+        <v>361</v>
+      </c>
+      <c r="R9" s="19" t="s">
+        <v>383</v>
+      </c>
       <c r="S9" t="s">
         <v>49</v>
       </c>
@@ -4037,32 +4304,38 @@
         <v>76</v>
       </c>
       <c r="AZ9">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA9">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC9" s="57"/>
       <c r="BD9" s="57"/>
       <c r="BE9" s="57"/>
       <c r="BF9" s="57"/>
-      <c r="BH9" s="66">
+      <c r="BH9" s="65">
         <v>41226</v>
       </c>
-      <c r="BI9" s="67" t="s">
+      <c r="BI9" s="66" t="s">
         <v>337</v>
       </c>
-      <c r="BJ9" s="25"/>
-      <c r="BK9" s="25"/>
-      <c r="BL9" t="s">
+      <c r="BJ9" s="67">
+        <v>31.671759999999999</v>
+      </c>
+      <c r="BK9" s="67">
+        <v>34.543559999999999</v>
+      </c>
+      <c r="BL9" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM9"/>
+      <c r="BM9" t="s">
+        <v>350</v>
+      </c>
       <c r="BN9" s="25"/>
       <c r="BS9">
         <v>5</v>
       </c>
-      <c r="BT9" s="69" t="s">
+      <c r="BT9" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU9"/>
@@ -4075,7 +4348,7 @@
     </row>
     <row r="10" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
-        <f>COUNTIF(D10,"&lt;&gt;"&amp;"")+COUNTIF(BN10,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B10" s="23">
@@ -4111,10 +4384,18 @@
       <c r="N10" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O10" s="37"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="19"/>
+      <c r="O10" s="37">
+        <v>137661</v>
+      </c>
+      <c r="P10" s="40">
+        <v>137661</v>
+      </c>
+      <c r="Q10" s="54" t="s">
+        <v>362</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>384</v>
+      </c>
       <c r="S10" t="s">
         <v>49</v>
       </c>
@@ -4203,32 +4484,38 @@
         <v>76</v>
       </c>
       <c r="AZ10">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA10">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC10" s="57"/>
       <c r="BD10" s="57"/>
       <c r="BE10" s="57"/>
       <c r="BF10" s="57"/>
-      <c r="BH10" s="66">
+      <c r="BH10" s="65">
         <v>41226</v>
       </c>
-      <c r="BI10" s="67" t="s">
+      <c r="BI10" s="66" t="s">
         <v>337</v>
       </c>
-      <c r="BJ10" s="25"/>
-      <c r="BK10" s="25"/>
-      <c r="BL10" t="s">
+      <c r="BJ10" s="67">
+        <v>31.671759999999999</v>
+      </c>
+      <c r="BK10" s="67">
+        <v>34.543559999999999</v>
+      </c>
+      <c r="BL10" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM10"/>
+      <c r="BM10" t="s">
+        <v>350</v>
+      </c>
       <c r="BN10" s="25"/>
       <c r="BS10">
         <v>5</v>
       </c>
-      <c r="BT10" s="69" t="s">
+      <c r="BT10" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU10"/>
@@ -4241,7 +4528,7 @@
     </row>
     <row r="11" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
-        <f>COUNTIF(D11,"&lt;&gt;"&amp;"")+COUNTIF(BN11,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B11" s="23">
@@ -4277,10 +4564,18 @@
       <c r="N11" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="37"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="54"/>
-      <c r="R11" s="19"/>
+      <c r="O11" s="37">
+        <v>273123</v>
+      </c>
+      <c r="P11" s="40">
+        <v>273123</v>
+      </c>
+      <c r="Q11" s="54" t="s">
+        <v>363</v>
+      </c>
+      <c r="R11" s="19" t="s">
+        <v>385</v>
+      </c>
       <c r="S11" t="s">
         <v>49</v>
       </c>
@@ -4369,32 +4664,38 @@
         <v>76</v>
       </c>
       <c r="AZ11">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA11">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC11" s="57"/>
       <c r="BD11" s="57"/>
       <c r="BE11" s="57"/>
       <c r="BF11" s="57"/>
-      <c r="BH11" s="66">
+      <c r="BH11" s="65">
         <v>41226</v>
       </c>
-      <c r="BI11" s="67" t="s">
+      <c r="BI11" s="66" t="s">
         <v>337</v>
       </c>
-      <c r="BJ11" s="25"/>
-      <c r="BK11" s="25"/>
-      <c r="BL11" t="s">
+      <c r="BJ11" s="67">
+        <v>31.671759999999999</v>
+      </c>
+      <c r="BK11" s="67">
+        <v>34.543559999999999</v>
+      </c>
+      <c r="BL11" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM11" s="58"/>
+      <c r="BM11" t="s">
+        <v>350</v>
+      </c>
       <c r="BN11" s="25"/>
       <c r="BS11">
         <v>5</v>
       </c>
-      <c r="BT11" s="69" t="s">
+      <c r="BT11" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU11"/>
@@ -4407,7 +4708,7 @@
     </row>
     <row r="12" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
-        <f>COUNTIF(D12,"&lt;&gt;"&amp;"")+COUNTIF(BN12,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B12" s="23">
@@ -4443,10 +4744,18 @@
       <c r="N12" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O12" s="37"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="24"/>
+      <c r="O12" s="37">
+        <v>134807</v>
+      </c>
+      <c r="P12" s="40">
+        <v>134807</v>
+      </c>
+      <c r="Q12" s="54" t="s">
+        <v>364</v>
+      </c>
+      <c r="R12" s="24" t="s">
+        <v>386</v>
+      </c>
       <c r="S12" t="s">
         <v>49</v>
       </c>
@@ -4535,32 +4844,38 @@
         <v>76</v>
       </c>
       <c r="AZ12">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA12">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC12" s="57"/>
       <c r="BD12" s="57"/>
       <c r="BE12" s="57"/>
       <c r="BF12" s="57"/>
-      <c r="BH12" s="66">
+      <c r="BH12" s="65">
         <v>41227</v>
       </c>
-      <c r="BI12" s="67" t="s">
+      <c r="BI12" s="66" t="s">
         <v>338</v>
       </c>
-      <c r="BJ12" s="25"/>
-      <c r="BK12" s="25"/>
-      <c r="BL12" t="s">
+      <c r="BJ12" s="67">
+        <v>31.941859999999998</v>
+      </c>
+      <c r="BK12" s="67">
+        <v>34.68862</v>
+      </c>
+      <c r="BL12" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM12" s="58"/>
+      <c r="BM12" s="58" t="s">
+        <v>351</v>
+      </c>
       <c r="BN12" s="25"/>
       <c r="BS12">
         <v>18</v>
       </c>
-      <c r="BT12" s="69" t="s">
+      <c r="BT12" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU12"/>
@@ -4573,7 +4888,7 @@
     </row>
     <row r="13" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
-        <f>COUNTIF(D13,"&lt;&gt;"&amp;"")+COUNTIF(BN13,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B13" s="23">
@@ -4609,10 +4924,18 @@
       <c r="N13" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O13" s="37"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="54"/>
-      <c r="R13" s="19"/>
+      <c r="O13" s="37">
+        <v>244784</v>
+      </c>
+      <c r="P13" s="40">
+        <v>244784</v>
+      </c>
+      <c r="Q13" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>387</v>
+      </c>
       <c r="S13" t="s">
         <v>49</v>
       </c>
@@ -4701,32 +5024,38 @@
         <v>76</v>
       </c>
       <c r="AZ13">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA13">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC13" s="57"/>
       <c r="BD13" s="57"/>
       <c r="BE13" s="57"/>
       <c r="BF13" s="57"/>
-      <c r="BH13" s="66">
+      <c r="BH13" s="65">
         <v>41227</v>
       </c>
-      <c r="BI13" s="67" t="s">
+      <c r="BI13" s="66" t="s">
         <v>338</v>
       </c>
-      <c r="BJ13" s="25"/>
-      <c r="BK13" s="25"/>
-      <c r="BL13" t="s">
+      <c r="BJ13" s="67">
+        <v>31.941859999999998</v>
+      </c>
+      <c r="BK13" s="67">
+        <v>34.68862</v>
+      </c>
+      <c r="BL13" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM13" s="58"/>
+      <c r="BM13" s="58" t="s">
+        <v>351</v>
+      </c>
       <c r="BN13" s="25"/>
       <c r="BS13">
         <v>18</v>
       </c>
-      <c r="BT13" s="69" t="s">
+      <c r="BT13" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU13"/>
@@ -4739,7 +5068,7 @@
     </row>
     <row r="14" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
-        <f>COUNTIF(D14,"&lt;&gt;"&amp;"")+COUNTIF(BN14,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B14" s="23">
@@ -4775,10 +5104,18 @@
       <c r="N14" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O14" s="37"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="55"/>
-      <c r="R14" s="19"/>
+      <c r="O14" s="37">
+        <v>337801</v>
+      </c>
+      <c r="P14" s="40">
+        <v>337801</v>
+      </c>
+      <c r="Q14" s="55" t="s">
+        <v>366</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>388</v>
+      </c>
       <c r="S14" t="s">
         <v>49</v>
       </c>
@@ -4867,32 +5204,38 @@
         <v>76</v>
       </c>
       <c r="AZ14">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA14">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC14" s="57"/>
       <c r="BD14" s="57"/>
       <c r="BE14" s="57"/>
       <c r="BF14" s="57"/>
-      <c r="BH14" s="66">
+      <c r="BH14" s="65">
         <v>41227</v>
       </c>
-      <c r="BI14" s="67" t="s">
+      <c r="BI14" s="66" t="s">
         <v>338</v>
       </c>
-      <c r="BJ14" s="25"/>
-      <c r="BK14" s="25"/>
-      <c r="BL14" t="s">
+      <c r="BJ14" s="67">
+        <v>31.941859999999998</v>
+      </c>
+      <c r="BK14" s="67">
+        <v>34.68862</v>
+      </c>
+      <c r="BL14" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM14" s="58"/>
+      <c r="BM14" s="58" t="s">
+        <v>351</v>
+      </c>
       <c r="BN14" s="25"/>
       <c r="BS14">
         <v>18</v>
       </c>
-      <c r="BT14" s="69" t="s">
+      <c r="BT14" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU14"/>
@@ -4905,7 +5248,7 @@
     </row>
     <row r="15" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
-        <f>COUNTIF(D15,"&lt;&gt;"&amp;"")+COUNTIF(BN15,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B15" s="23">
@@ -4941,10 +5284,18 @@
       <c r="N15" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O15" s="37"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="19"/>
+      <c r="O15" s="37">
+        <v>252074</v>
+      </c>
+      <c r="P15" s="40">
+        <v>252074</v>
+      </c>
+      <c r="Q15" s="54" t="s">
+        <v>367</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>389</v>
+      </c>
       <c r="S15" t="s">
         <v>49</v>
       </c>
@@ -5033,32 +5384,38 @@
         <v>76</v>
       </c>
       <c r="AZ15">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA15">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC15" s="57"/>
       <c r="BD15" s="57"/>
       <c r="BE15" s="57"/>
       <c r="BF15" s="57"/>
-      <c r="BH15" s="66">
+      <c r="BH15" s="65">
         <v>41227</v>
       </c>
-      <c r="BI15" s="67" t="s">
+      <c r="BI15" s="66" t="s">
         <v>339</v>
       </c>
-      <c r="BJ15" s="25"/>
-      <c r="BK15" s="25"/>
-      <c r="BL15" t="s">
+      <c r="BJ15" s="67">
+        <v>31.94068</v>
+      </c>
+      <c r="BK15" s="67">
+        <v>34.687379999999997</v>
+      </c>
+      <c r="BL15" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM15" s="58"/>
+      <c r="BM15" s="58" t="s">
+        <v>351</v>
+      </c>
       <c r="BN15" s="25"/>
       <c r="BS15">
         <v>19</v>
       </c>
-      <c r="BT15" s="69" t="s">
+      <c r="BT15" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU15"/>
@@ -5071,7 +5428,7 @@
     </row>
     <row r="16" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
-        <f>COUNTIF(D16,"&lt;&gt;"&amp;"")+COUNTIF(BN16,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B16" s="23">
@@ -5105,10 +5462,21 @@
         <v>250</v>
       </c>
       <c r="N16" s="30"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="40"/>
-      <c r="Q16" s="54"/>
-      <c r="R16" s="19"/>
+      <c r="O16" s="37">
+        <v>154501</v>
+      </c>
+      <c r="P16" s="40">
+        <v>154501</v>
+      </c>
+      <c r="Q16" s="54" t="s">
+        <v>368</v>
+      </c>
+      <c r="R16" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="S16" t="s">
+        <v>49</v>
+      </c>
       <c r="T16" s="16" t="s">
         <v>180</v>
       </c>
@@ -5189,32 +5557,38 @@
         <v>76</v>
       </c>
       <c r="AZ16">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA16">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC16" s="57"/>
       <c r="BD16" s="57"/>
       <c r="BE16" s="57"/>
       <c r="BF16" s="57"/>
-      <c r="BH16" s="66">
+      <c r="BH16" s="65">
         <v>41227</v>
       </c>
-      <c r="BI16" s="67" t="s">
+      <c r="BI16" s="66" t="s">
         <v>339</v>
       </c>
-      <c r="BJ16" s="25"/>
-      <c r="BK16" s="25"/>
-      <c r="BL16" t="s">
+      <c r="BJ16" s="67">
+        <v>31.94068</v>
+      </c>
+      <c r="BK16" s="67">
+        <v>34.687379999999997</v>
+      </c>
+      <c r="BL16" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM16" s="58"/>
+      <c r="BM16" s="58" t="s">
+        <v>351</v>
+      </c>
       <c r="BN16" s="25"/>
       <c r="BS16">
         <v>19</v>
       </c>
-      <c r="BT16" s="69" t="s">
+      <c r="BT16" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU16"/>
@@ -5227,7 +5601,7 @@
     </row>
     <row r="17" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
-        <f>COUNTIF(D17,"&lt;&gt;"&amp;"")+COUNTIF(BN17,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B17" s="23">
@@ -5261,10 +5635,21 @@
         <v>250</v>
       </c>
       <c r="N17" s="30"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="55"/>
-      <c r="R17" s="19"/>
+      <c r="O17" s="37">
+        <v>174238</v>
+      </c>
+      <c r="P17" s="40">
+        <v>174238</v>
+      </c>
+      <c r="Q17" s="55" t="s">
+        <v>369</v>
+      </c>
+      <c r="R17" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="S17" t="s">
+        <v>49</v>
+      </c>
       <c r="T17" s="16" t="s">
         <v>181</v>
       </c>
@@ -5345,32 +5730,38 @@
         <v>76</v>
       </c>
       <c r="AZ17">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA17">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC17" s="57"/>
       <c r="BD17" s="57"/>
       <c r="BE17" s="57"/>
       <c r="BF17" s="57"/>
-      <c r="BH17" s="66">
+      <c r="BH17" s="65">
         <v>41227</v>
       </c>
-      <c r="BI17" s="67" t="s">
+      <c r="BI17" s="66" t="s">
         <v>339</v>
       </c>
-      <c r="BJ17" s="25"/>
-      <c r="BK17" s="25"/>
-      <c r="BL17" t="s">
+      <c r="BJ17" s="67">
+        <v>31.94068</v>
+      </c>
+      <c r="BK17" s="67">
+        <v>34.687379999999997</v>
+      </c>
+      <c r="BL17" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM17" s="58"/>
+      <c r="BM17" s="58" t="s">
+        <v>351</v>
+      </c>
       <c r="BN17" s="25"/>
       <c r="BS17">
         <v>19</v>
       </c>
-      <c r="BT17" s="69" t="s">
+      <c r="BT17" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU17"/>
@@ -5383,7 +5774,7 @@
     </row>
     <row r="18" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
-        <f>COUNTIF(D18,"&lt;&gt;"&amp;"")+COUNTIF(BN18,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B18" s="23">
@@ -5417,10 +5808,21 @@
         <v>250</v>
       </c>
       <c r="N18" s="30"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="19"/>
+      <c r="O18" s="37">
+        <v>171763</v>
+      </c>
+      <c r="P18" s="40">
+        <v>171763</v>
+      </c>
+      <c r="Q18" s="54" t="s">
+        <v>370</v>
+      </c>
+      <c r="R18" s="19" t="s">
+        <v>392</v>
+      </c>
+      <c r="S18" t="s">
+        <v>49</v>
+      </c>
       <c r="T18" s="16" t="s">
         <v>182</v>
       </c>
@@ -5501,32 +5903,38 @@
         <v>76</v>
       </c>
       <c r="AZ18">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA18">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC18" s="57"/>
       <c r="BD18" s="57"/>
       <c r="BE18" s="57"/>
       <c r="BF18" s="57"/>
-      <c r="BH18" s="66">
+      <c r="BH18" s="65">
         <v>41227</v>
       </c>
-      <c r="BI18" s="67" t="s">
+      <c r="BI18" s="66" t="s">
         <v>340</v>
       </c>
-      <c r="BJ18" s="25"/>
-      <c r="BK18" s="25"/>
-      <c r="BL18" t="s">
+      <c r="BJ18" s="67">
+        <v>31.931660000000001</v>
+      </c>
+      <c r="BK18" s="67">
+        <v>34.68336</v>
+      </c>
+      <c r="BL18" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM18" s="58"/>
+      <c r="BM18" s="58" t="s">
+        <v>352</v>
+      </c>
       <c r="BN18" s="25"/>
       <c r="BS18">
         <v>18</v>
       </c>
-      <c r="BT18" s="69" t="s">
+      <c r="BT18" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU18"/>
@@ -5539,7 +5947,7 @@
     </row>
     <row r="19" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
-        <f>COUNTIF(D19,"&lt;&gt;"&amp;"")+COUNTIF(BN19,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B19" s="23">
@@ -5573,10 +5981,21 @@
         <v>250</v>
       </c>
       <c r="N19" s="30"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="54"/>
-      <c r="R19" s="19"/>
+      <c r="O19" s="37">
+        <v>237422</v>
+      </c>
+      <c r="P19" s="40">
+        <v>237422</v>
+      </c>
+      <c r="Q19" s="54" t="s">
+        <v>371</v>
+      </c>
+      <c r="R19" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="S19" t="s">
+        <v>49</v>
+      </c>
       <c r="T19" s="16" t="s">
         <v>183</v>
       </c>
@@ -5657,32 +6076,38 @@
         <v>76</v>
       </c>
       <c r="AZ19">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA19">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC19" s="57"/>
       <c r="BD19" s="57"/>
       <c r="BE19" s="57"/>
       <c r="BF19" s="57"/>
-      <c r="BH19" s="66">
+      <c r="BH19" s="65">
         <v>41227</v>
       </c>
-      <c r="BI19" s="67" t="s">
+      <c r="BI19" s="66" t="s">
         <v>340</v>
       </c>
-      <c r="BJ19" s="25"/>
-      <c r="BK19" s="25"/>
-      <c r="BL19" t="s">
+      <c r="BJ19" s="67">
+        <v>31.931660000000001</v>
+      </c>
+      <c r="BK19" s="67">
+        <v>34.68336</v>
+      </c>
+      <c r="BL19" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM19"/>
+      <c r="BM19" t="s">
+        <v>352</v>
+      </c>
       <c r="BN19" s="25"/>
       <c r="BS19">
         <v>18</v>
       </c>
-      <c r="BT19" s="69" t="s">
+      <c r="BT19" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU19"/>
@@ -5695,7 +6120,7 @@
     </row>
     <row r="20" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
-        <f>COUNTIF(D20,"&lt;&gt;"&amp;"")+COUNTIF(BN20,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B20" s="23">
@@ -5729,10 +6154,21 @@
         <v>250</v>
       </c>
       <c r="N20" s="30"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="54"/>
-      <c r="R20" s="19"/>
+      <c r="O20" s="37">
+        <v>154346</v>
+      </c>
+      <c r="P20" s="40">
+        <v>154346</v>
+      </c>
+      <c r="Q20" s="54" t="s">
+        <v>372</v>
+      </c>
+      <c r="R20" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="S20" t="s">
+        <v>49</v>
+      </c>
       <c r="T20" s="16" t="s">
         <v>184</v>
       </c>
@@ -5813,32 +6249,38 @@
         <v>76</v>
       </c>
       <c r="AZ20">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA20">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC20" s="57"/>
       <c r="BD20" s="57"/>
       <c r="BE20" s="57"/>
       <c r="BF20" s="57"/>
-      <c r="BH20" s="66">
+      <c r="BH20" s="65">
         <v>41227</v>
       </c>
-      <c r="BI20" s="67" t="s">
+      <c r="BI20" s="66" t="s">
         <v>340</v>
       </c>
-      <c r="BJ20" s="25"/>
-      <c r="BK20" s="25"/>
-      <c r="BL20" t="s">
+      <c r="BJ20" s="67">
+        <v>31.931660000000001</v>
+      </c>
+      <c r="BK20" s="67">
+        <v>34.68336</v>
+      </c>
+      <c r="BL20" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM20"/>
+      <c r="BM20" t="s">
+        <v>352</v>
+      </c>
       <c r="BN20" s="25"/>
       <c r="BS20">
         <v>18</v>
       </c>
-      <c r="BT20" s="69" t="s">
+      <c r="BT20" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU20"/>
@@ -5851,7 +6293,7 @@
     </row>
     <row r="21" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
-        <f>COUNTIF(D21,"&lt;&gt;"&amp;"")+COUNTIF(BN21,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B21" s="23">
@@ -5885,10 +6327,17 @@
         <v>250</v>
       </c>
       <c r="N21" s="30"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="40"/>
+      <c r="O21" s="37">
+        <v>0</v>
+      </c>
+      <c r="P21" s="40">
+        <v>0</v>
+      </c>
       <c r="Q21" s="54"/>
       <c r="R21" s="19"/>
+      <c r="S21" t="s">
+        <v>49</v>
+      </c>
       <c r="T21" s="16" t="s">
         <v>191</v>
       </c>
@@ -5969,32 +6418,38 @@
         <v>76</v>
       </c>
       <c r="AZ21">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA21">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC21" s="57"/>
       <c r="BD21" s="57"/>
       <c r="BE21" s="57"/>
       <c r="BF21" s="57"/>
-      <c r="BH21" s="66">
+      <c r="BH21" s="65">
         <v>41233</v>
       </c>
-      <c r="BI21" s="67" t="s">
+      <c r="BI21" s="66" t="s">
         <v>341</v>
       </c>
-      <c r="BJ21" s="25"/>
-      <c r="BK21" s="25"/>
-      <c r="BL21" t="s">
+      <c r="BJ21" s="67">
+        <v>32.465020000000003</v>
+      </c>
+      <c r="BK21" s="67">
+        <v>34.882582999999997</v>
+      </c>
+      <c r="BL21" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM21"/>
+      <c r="BM21" s="58" t="s">
+        <v>353</v>
+      </c>
       <c r="BN21" s="25"/>
       <c r="BS21">
         <v>3.8</v>
       </c>
-      <c r="BT21" t="s">
+      <c r="BT21" s="42" t="s">
         <v>345</v>
       </c>
       <c r="BU21"/>
@@ -6007,7 +6462,7 @@
     </row>
     <row r="22" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
-        <f>COUNTIF(D22,"&lt;&gt;"&amp;"")+COUNTIF(BN22,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B22" s="23">
@@ -6041,10 +6496,21 @@
         <v>250</v>
       </c>
       <c r="N22" s="30"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="54"/>
-      <c r="R22" s="19"/>
+      <c r="O22" s="37">
+        <v>356730</v>
+      </c>
+      <c r="P22" s="40">
+        <v>356730</v>
+      </c>
+      <c r="Q22" s="54" t="s">
+        <v>373</v>
+      </c>
+      <c r="R22" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="S22" t="s">
+        <v>49</v>
+      </c>
       <c r="T22" s="16" t="s">
         <v>185</v>
       </c>
@@ -6125,32 +6591,38 @@
         <v>76</v>
       </c>
       <c r="AZ22">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA22">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC22" s="57"/>
       <c r="BD22" s="57"/>
       <c r="BE22" s="57"/>
       <c r="BF22" s="57"/>
-      <c r="BH22" s="66">
+      <c r="BH22" s="65">
         <v>41233</v>
       </c>
-      <c r="BI22" s="67" t="s">
+      <c r="BI22" s="66" t="s">
         <v>341</v>
       </c>
-      <c r="BJ22" s="25"/>
-      <c r="BK22" s="25"/>
-      <c r="BL22" t="s">
+      <c r="BJ22" s="67">
+        <v>32.465020000000003</v>
+      </c>
+      <c r="BK22" s="67">
+        <v>34.882582999999997</v>
+      </c>
+      <c r="BL22" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM22"/>
+      <c r="BM22" s="58" t="s">
+        <v>353</v>
+      </c>
       <c r="BN22" s="25"/>
       <c r="BS22">
         <v>3.8</v>
       </c>
-      <c r="BT22" t="s">
+      <c r="BT22" s="42" t="s">
         <v>345</v>
       </c>
       <c r="BU22"/>
@@ -6163,7 +6635,7 @@
     </row>
     <row r="23" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
-        <f>COUNTIF(D23,"&lt;&gt;"&amp;"")+COUNTIF(BN23,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B23" s="23">
@@ -6197,10 +6669,21 @@
         <v>250</v>
       </c>
       <c r="N23" s="30"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="40"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="19"/>
+      <c r="O23" s="37">
+        <v>406279</v>
+      </c>
+      <c r="P23" s="40">
+        <v>406279</v>
+      </c>
+      <c r="Q23" s="54" t="s">
+        <v>374</v>
+      </c>
+      <c r="R23" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="S23" t="s">
+        <v>49</v>
+      </c>
       <c r="T23" s="16" t="s">
         <v>186</v>
       </c>
@@ -6281,32 +6764,38 @@
         <v>76</v>
       </c>
       <c r="AZ23">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA23">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC23" s="57"/>
       <c r="BD23" s="57"/>
       <c r="BE23" s="57"/>
       <c r="BF23" s="57"/>
-      <c r="BH23" s="66">
+      <c r="BH23" s="65">
         <v>41233</v>
       </c>
-      <c r="BI23" s="67" t="s">
+      <c r="BI23" s="66" t="s">
         <v>341</v>
       </c>
-      <c r="BJ23" s="25"/>
-      <c r="BK23" s="25"/>
-      <c r="BL23" t="s">
+      <c r="BJ23" s="67">
+        <v>32.465020000000003</v>
+      </c>
+      <c r="BK23" s="67">
+        <v>34.882582999999997</v>
+      </c>
+      <c r="BL23" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM23"/>
+      <c r="BM23" s="58" t="s">
+        <v>353</v>
+      </c>
       <c r="BN23" s="25"/>
       <c r="BS23">
         <v>3.8</v>
       </c>
-      <c r="BT23" t="s">
+      <c r="BT23" s="42" t="s">
         <v>345</v>
       </c>
       <c r="BU23"/>
@@ -6319,7 +6808,7 @@
     </row>
     <row r="24" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
-        <f>COUNTIF(D24,"&lt;&gt;"&amp;"")+COUNTIF(BN24,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B24" s="23">
@@ -6353,10 +6842,21 @@
         <v>250</v>
       </c>
       <c r="N24" s="30"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="19"/>
+      <c r="O24" s="37">
+        <v>292338</v>
+      </c>
+      <c r="P24" s="40">
+        <v>292338</v>
+      </c>
+      <c r="Q24" s="54" t="s">
+        <v>375</v>
+      </c>
+      <c r="R24" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="S24" t="s">
+        <v>49</v>
+      </c>
       <c r="T24" s="16" t="s">
         <v>187</v>
       </c>
@@ -6437,32 +6937,38 @@
         <v>76</v>
       </c>
       <c r="AZ24">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA24">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC24" s="57"/>
       <c r="BD24" s="57"/>
       <c r="BE24" s="57"/>
       <c r="BF24" s="57"/>
-      <c r="BH24" s="66">
+      <c r="BH24" s="65">
         <v>41233</v>
       </c>
-      <c r="BI24" s="67" t="s">
+      <c r="BI24" s="66" t="s">
         <v>342</v>
       </c>
-      <c r="BJ24" s="25"/>
-      <c r="BK24" s="25"/>
-      <c r="BL24" t="s">
+      <c r="BJ24" s="67">
+        <v>32.463700000000003</v>
+      </c>
+      <c r="BK24" s="67">
+        <v>34.879339999999999</v>
+      </c>
+      <c r="BL24" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM24"/>
+      <c r="BM24" s="58" t="s">
+        <v>355</v>
+      </c>
       <c r="BN24" s="25"/>
       <c r="BS24">
         <v>5.5</v>
       </c>
-      <c r="BT24" s="69" t="s">
+      <c r="BT24" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU24"/>
@@ -6475,7 +6981,7 @@
     </row>
     <row r="25" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
-        <f>COUNTIF(D25,"&lt;&gt;"&amp;"")+COUNTIF(BN25,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B25" s="23">
@@ -6509,10 +7015,21 @@
         <v>250</v>
       </c>
       <c r="N25" s="30"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="19"/>
+      <c r="O25" s="37">
+        <v>269103</v>
+      </c>
+      <c r="P25" s="40">
+        <v>269103</v>
+      </c>
+      <c r="Q25" s="54" t="s">
+        <v>376</v>
+      </c>
+      <c r="R25" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="S25" t="s">
+        <v>49</v>
+      </c>
       <c r="T25" s="16" t="s">
         <v>188</v>
       </c>
@@ -6593,32 +7110,38 @@
         <v>76</v>
       </c>
       <c r="AZ25">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA25">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC25" s="57"/>
       <c r="BD25" s="57"/>
       <c r="BE25" s="57"/>
       <c r="BF25" s="57"/>
-      <c r="BH25" s="66">
+      <c r="BH25" s="65">
         <v>41233</v>
       </c>
-      <c r="BI25" s="67" t="s">
+      <c r="BI25" s="66" t="s">
         <v>342</v>
       </c>
-      <c r="BJ25" s="25"/>
-      <c r="BK25" s="25"/>
-      <c r="BL25" t="s">
+      <c r="BJ25" s="67">
+        <v>32.463700000000003</v>
+      </c>
+      <c r="BK25" s="67">
+        <v>34.879339999999999</v>
+      </c>
+      <c r="BL25" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM25"/>
+      <c r="BM25" s="58" t="s">
+        <v>355</v>
+      </c>
       <c r="BN25" s="25"/>
       <c r="BS25">
         <v>5.5</v>
       </c>
-      <c r="BT25" s="69" t="s">
+      <c r="BT25" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU25"/>
@@ -6631,7 +7154,7 @@
     </row>
     <row r="26" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
-        <f>COUNTIF(D26,"&lt;&gt;"&amp;"")+COUNTIF(BN26,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B26" s="23">
@@ -6665,10 +7188,17 @@
         <v>250</v>
       </c>
       <c r="N26" s="30"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="40"/>
+      <c r="O26" s="37">
+        <v>0</v>
+      </c>
+      <c r="P26" s="40">
+        <v>0</v>
+      </c>
       <c r="Q26" s="54"/>
       <c r="R26" s="19"/>
+      <c r="S26" t="s">
+        <v>49</v>
+      </c>
       <c r="T26" s="16" t="s">
         <v>192</v>
       </c>
@@ -6749,32 +7279,38 @@
         <v>76</v>
       </c>
       <c r="AZ26">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA26">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC26" s="57"/>
       <c r="BD26" s="57"/>
       <c r="BE26" s="57"/>
       <c r="BF26" s="57"/>
-      <c r="BH26" s="66">
+      <c r="BH26" s="65">
         <v>41233</v>
       </c>
-      <c r="BI26" s="67" t="s">
+      <c r="BI26" s="66" t="s">
         <v>342</v>
       </c>
-      <c r="BJ26" s="25"/>
-      <c r="BK26" s="25"/>
-      <c r="BL26" t="s">
+      <c r="BJ26" s="67">
+        <v>32.463700000000003</v>
+      </c>
+      <c r="BK26" s="67">
+        <v>34.879339999999999</v>
+      </c>
+      <c r="BL26" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM26"/>
+      <c r="BM26" s="58" t="s">
+        <v>355</v>
+      </c>
       <c r="BN26" s="25"/>
       <c r="BS26">
         <v>5.5</v>
       </c>
-      <c r="BT26" s="69" t="s">
+      <c r="BT26" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU26"/>
@@ -6787,7 +7323,7 @@
     </row>
     <row r="27" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
-        <f>COUNTIF(D27,"&lt;&gt;"&amp;"")+COUNTIF(BN27,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B27" s="23">
@@ -6821,10 +7357,21 @@
         <v>250</v>
       </c>
       <c r="N27" s="30"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="54"/>
-      <c r="R27" s="19"/>
+      <c r="O27" s="37">
+        <v>190462</v>
+      </c>
+      <c r="P27" s="40">
+        <v>190462</v>
+      </c>
+      <c r="Q27" s="54" t="s">
+        <v>377</v>
+      </c>
+      <c r="R27" s="19" t="s">
+        <v>399</v>
+      </c>
+      <c r="S27" t="s">
+        <v>49</v>
+      </c>
       <c r="T27" s="16" t="s">
         <v>189</v>
       </c>
@@ -6905,32 +7452,38 @@
         <v>76</v>
       </c>
       <c r="AZ27">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA27">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC27" s="57"/>
       <c r="BD27" s="57"/>
       <c r="BE27" s="57"/>
       <c r="BF27" s="57"/>
-      <c r="BH27" s="66">
+      <c r="BH27" s="65">
         <v>41233</v>
       </c>
-      <c r="BI27" s="67" t="s">
+      <c r="BI27" s="66" t="s">
         <v>343</v>
       </c>
-      <c r="BJ27" s="25"/>
-      <c r="BK27" s="25"/>
-      <c r="BL27" t="s">
+      <c r="BJ27" s="67">
+        <v>32.42868</v>
+      </c>
+      <c r="BK27" s="67">
+        <v>34.870280000000001</v>
+      </c>
+      <c r="BL27" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM27"/>
+      <c r="BM27" t="s">
+        <v>354</v>
+      </c>
       <c r="BN27" s="25"/>
       <c r="BS27">
         <v>6.5</v>
       </c>
-      <c r="BT27" s="69" t="s">
+      <c r="BT27" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU27"/>
@@ -6943,7 +7496,7 @@
     </row>
     <row r="28" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A28" s="12">
-        <f>COUNTIF(D28,"&lt;&gt;"&amp;"")+COUNTIF(BN28,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B28" s="23">
@@ -6977,10 +7530,17 @@
         <v>250</v>
       </c>
       <c r="N28" s="30"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="40"/>
+      <c r="O28" s="37">
+        <v>0</v>
+      </c>
+      <c r="P28" s="40">
+        <v>0</v>
+      </c>
       <c r="Q28" s="54"/>
       <c r="R28" s="19"/>
+      <c r="S28" t="s">
+        <v>49</v>
+      </c>
       <c r="T28" s="16" t="s">
         <v>193</v>
       </c>
@@ -7061,32 +7621,38 @@
         <v>76</v>
       </c>
       <c r="AZ28">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA28">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC28" s="57"/>
       <c r="BD28" s="57"/>
       <c r="BE28" s="57"/>
       <c r="BF28" s="57"/>
-      <c r="BH28" s="66">
+      <c r="BH28" s="65">
         <v>41233</v>
       </c>
-      <c r="BI28" s="67" t="s">
+      <c r="BI28" s="66" t="s">
         <v>343</v>
       </c>
-      <c r="BJ28" s="25"/>
-      <c r="BK28" s="25"/>
-      <c r="BL28" t="s">
+      <c r="BJ28" s="67">
+        <v>32.42868</v>
+      </c>
+      <c r="BK28" s="67">
+        <v>34.870280000000001</v>
+      </c>
+      <c r="BL28" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM28"/>
+      <c r="BM28" t="s">
+        <v>354</v>
+      </c>
       <c r="BN28" s="25"/>
       <c r="BS28">
         <v>6.5</v>
       </c>
-      <c r="BT28" s="69" t="s">
+      <c r="BT28" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU28"/>
@@ -7099,7 +7665,7 @@
     </row>
     <row r="29" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
-        <f>COUNTIF(D29,"&lt;&gt;"&amp;"")+COUNTIF(BN29,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B29" s="23">
@@ -7133,10 +7699,17 @@
         <v>250</v>
       </c>
       <c r="N29" s="30"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="40"/>
+      <c r="O29" s="37">
+        <v>0</v>
+      </c>
+      <c r="P29" s="40">
+        <v>0</v>
+      </c>
       <c r="Q29" s="54"/>
       <c r="R29" s="19"/>
+      <c r="S29" t="s">
+        <v>49</v>
+      </c>
       <c r="T29" s="16" t="s">
         <v>194</v>
       </c>
@@ -7217,32 +7790,38 @@
         <v>76</v>
       </c>
       <c r="AZ29">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA29">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BC29" s="57"/>
       <c r="BD29" s="57"/>
       <c r="BE29" s="57"/>
       <c r="BF29" s="57"/>
-      <c r="BH29" s="66">
+      <c r="BH29" s="65">
         <v>41233</v>
       </c>
-      <c r="BI29" s="67" t="s">
+      <c r="BI29" s="66" t="s">
         <v>343</v>
       </c>
-      <c r="BJ29" s="25"/>
-      <c r="BK29" s="25"/>
-      <c r="BL29" t="s">
+      <c r="BJ29" s="67">
+        <v>32.42868</v>
+      </c>
+      <c r="BK29" s="67">
+        <v>34.870280000000001</v>
+      </c>
+      <c r="BL29" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="BM29"/>
+      <c r="BM29" t="s">
+        <v>354</v>
+      </c>
       <c r="BN29" s="25"/>
       <c r="BS29">
         <v>6.5</v>
       </c>
-      <c r="BT29" s="69" t="s">
+      <c r="BT29" s="71" t="s">
         <v>346</v>
       </c>
       <c r="BU29"/>
@@ -7261,60 +7840,78 @@
     </row>
     <row r="32" spans="1:79" x14ac:dyDescent="0.2">
       <c r="AK32" s="13"/>
-      <c r="BI32" s="67"/>
+      <c r="BI32" s="66"/>
     </row>
-    <row r="33" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="33" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK33" s="13"/>
-      <c r="BI33" s="67"/>
+      <c r="BI33" s="66"/>
+      <c r="BM33" s="67"/>
+      <c r="BN33" s="67"/>
     </row>
-    <row r="34" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="34" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK34" s="13"/>
-      <c r="BI34" s="67"/>
+      <c r="BI34" s="66"/>
+      <c r="BM34" s="67"/>
+      <c r="BN34" s="67"/>
     </row>
-    <row r="35" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="35" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK35" s="13"/>
-      <c r="BI35" s="67"/>
+      <c r="BI35" s="66"/>
+      <c r="BM35" s="67"/>
+      <c r="BN35" s="67"/>
     </row>
-    <row r="36" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="36" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK36" s="13"/>
-      <c r="BI36" s="67"/>
+      <c r="BI36" s="66"/>
+      <c r="BM36" s="67"/>
+      <c r="BN36" s="67"/>
     </row>
-    <row r="37" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="37" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK37" s="13"/>
-      <c r="BI37" s="67"/>
+      <c r="BI37" s="66"/>
+      <c r="BM37" s="67"/>
+      <c r="BN37" s="67"/>
     </row>
-    <row r="38" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="38" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK38" s="13"/>
-      <c r="BI38" s="67"/>
+      <c r="BI38" s="66"/>
+      <c r="BM38" s="67"/>
+      <c r="BN38" s="67"/>
     </row>
-    <row r="39" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="39" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK39" s="13"/>
+      <c r="BM39" s="67"/>
+      <c r="BN39" s="67"/>
     </row>
-    <row r="40" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="40" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK40" s="13"/>
+      <c r="BM40" s="67"/>
+      <c r="BN40" s="67"/>
     </row>
-    <row r="41" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="41" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK41" s="13"/>
+      <c r="BM41" s="67"/>
+      <c r="BN41" s="67"/>
     </row>
-    <row r="42" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="42" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK42" s="13"/>
     </row>
-    <row r="43" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="43" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK43" s="13"/>
     </row>
-    <row r="44" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="44" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK44" s="13"/>
     </row>
-    <row r="45" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="45" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK45" s="13"/>
     </row>
-    <row r="46" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="46" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK46" s="13"/>
     </row>
-    <row r="47" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="47" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK47" s="13"/>
     </row>
-    <row r="48" spans="37:61" x14ac:dyDescent="0.2">
+    <row r="48" spans="37:66" x14ac:dyDescent="0.2">
       <c r="AK48" s="13"/>
     </row>
     <row r="49" spans="37:37" x14ac:dyDescent="0.2">
@@ -7328,9 +7925,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -7348,24 +7955,14 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Updating metadata for desalt
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/unige/desalt/metadata.xlsx
+++ b/metadata/excel/projects/unige/desalt/metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="340" yWindow="660" windowWidth="44080" windowHeight="25000" tabRatio="500"/>
+    <workbookView xWindow="660" yWindow="980" windowWidth="44080" windowHeight="25000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="micans_v6_ex1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="412">
   <si>
     <t>Country</t>
   </si>
@@ -885,12 +885,6 @@
     <t>Multiplexed in</t>
   </si>
   <si>
-    <t>SSUFO4</t>
-  </si>
-  <si>
-    <t>SSUR22</t>
-  </si>
-  <si>
     <t>V1V2 nSSU rDNA (18S rDNA)</t>
   </si>
   <si>
@@ -1357,6 +1351,18 @@
   </si>
   <si>
     <t>Distance to exhaust [m]</t>
+  </si>
+  <si>
+    <t>SSUF04</t>
+  </si>
+  <si>
+    <t>SSUR22mod</t>
+  </si>
+  <si>
+    <t>Grain size mode [µm]</t>
+  </si>
+  <si>
+    <t>Salinty [ppt]</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1372,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1512,18 +1518,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Menlo Regular"/>
     </font>
@@ -1540,6 +1534,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1906,7 +1906,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2046,14 +2046,12 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2065,10 +2063,10 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="291" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="291" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2077,6 +2075,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="304">
     <cellStyle name="Excel Built-in Normal" xfId="267"/>
@@ -2751,12 +2751,12 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:CG51"/>
+  <dimension ref="A1:CI51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BL1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="CA24" sqref="CA24"/>
+      <selection pane="bottomLeft" activeCell="CB23" sqref="CB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2823,7 +2823,7 @@
     <col min="64" max="65" width="15.5" customWidth="1"/>
     <col min="66" max="66" width="13.6640625" style="11" customWidth="1"/>
     <col min="67" max="67" width="13.1640625" style="11" customWidth="1"/>
-    <col min="68" max="68" width="13.1640625" style="68" customWidth="1"/>
+    <col min="68" max="68" width="13.1640625" style="66" customWidth="1"/>
     <col min="69" max="69" width="28" style="16" customWidth="1"/>
     <col min="70" max="70" width="31.33203125" style="16" customWidth="1"/>
     <col min="71" max="71" width="9" customWidth="1"/>
@@ -2831,19 +2831,20 @@
     <col min="73" max="73" width="16" customWidth="1"/>
     <col min="74" max="74" width="9.5" customWidth="1"/>
     <col min="75" max="75" width="11" style="22" customWidth="1"/>
-    <col min="76" max="76" width="11" style="72" customWidth="1"/>
-    <col min="77" max="77" width="13" style="72" customWidth="1"/>
-    <col min="78" max="78" width="11.6640625" style="22" customWidth="1"/>
-    <col min="79" max="79" width="14.33203125" style="22" customWidth="1"/>
+    <col min="76" max="76" width="11" style="70" customWidth="1"/>
+    <col min="77" max="77" width="13" style="70" customWidth="1"/>
+    <col min="78" max="79" width="11.6640625" style="22" customWidth="1"/>
     <col min="80" max="80" width="12.6640625" style="22" customWidth="1"/>
-    <col min="81" max="81" width="13.6640625" style="22" customWidth="1"/>
-    <col min="82" max="82" width="15.33203125" style="22" customWidth="1"/>
-    <col min="83" max="83" width="15.5" style="22" customWidth="1"/>
-    <col min="84" max="84" width="14.6640625" style="22" customWidth="1"/>
-    <col min="85" max="85" width="9.6640625" customWidth="1"/>
+    <col min="81" max="81" width="14.33203125" style="22" customWidth="1"/>
+    <col min="82" max="82" width="13.5" style="22" customWidth="1"/>
+    <col min="83" max="83" width="13.6640625" style="22" customWidth="1"/>
+    <col min="84" max="84" width="15.33203125" style="22" customWidth="1"/>
+    <col min="85" max="85" width="15.5" style="22" customWidth="1"/>
+    <col min="86" max="86" width="14.6640625" style="22" customWidth="1"/>
+    <col min="87" max="87" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -2895,30 +2896,30 @@
       <c r="BC1" s="3"/>
       <c r="BD1" s="3"/>
       <c r="BE1" s="10"/>
-      <c r="BG1" s="73" t="s">
+      <c r="BG1" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="BH1" s="73"/>
-      <c r="BI1" s="73"/>
-      <c r="BJ1" s="73"/>
-      <c r="BL1" s="73" t="s">
+      <c r="BH1" s="71"/>
+      <c r="BI1" s="71"/>
+      <c r="BJ1" s="71"/>
+      <c r="BL1" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="BM1" s="73"/>
-      <c r="BN1" s="73"/>
-      <c r="BO1" s="73"/>
-      <c r="BP1" s="73"/>
-      <c r="BQ1" s="73"/>
-      <c r="BR1" s="73"/>
-      <c r="BT1" s="73" t="s">
+      <c r="BM1" s="71"/>
+      <c r="BN1" s="71"/>
+      <c r="BO1" s="71"/>
+      <c r="BP1" s="71"/>
+      <c r="BQ1" s="71"/>
+      <c r="BR1" s="71"/>
+      <c r="BT1" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="BU1" s="73"/>
+      <c r="BU1" s="71"/>
       <c r="BW1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="BX1" s="69"/>
-      <c r="BY1" s="69"/>
+      <c r="BX1" s="67"/>
+      <c r="BY1" s="67"/>
       <c r="BZ1" s="21"/>
       <c r="CA1" s="21"/>
       <c r="CB1" s="21"/>
@@ -2926,8 +2927,10 @@
       <c r="CD1" s="21"/>
       <c r="CE1" s="21"/>
       <c r="CF1" s="21"/>
+      <c r="CG1" s="21"/>
+      <c r="CH1" s="21"/>
     </row>
-    <row r="2" spans="1:85" s="53" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:87" s="53" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
         <v>49</v>
       </c>
@@ -2987,13 +2990,13 @@
       </c>
       <c r="V2" s="45"/>
       <c r="W2" s="43" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="X2" s="43" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="Y2" s="43" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="Z2" s="45"/>
       <c r="AA2" s="43" t="s">
@@ -3101,7 +3104,7 @@
         <v>50</v>
       </c>
       <c r="BM2" s="50" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="BN2" s="50" t="s">
         <v>12</v>
@@ -3130,35 +3133,41 @@
         <v>28</v>
       </c>
       <c r="BX2" s="52" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="BY2" s="52" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="BZ2" s="52" t="s">
         <v>29</v>
       </c>
       <c r="CA2" s="52" t="s">
-        <v>42</v>
+        <v>411</v>
       </c>
       <c r="CB2" s="52" t="s">
         <v>31</v>
       </c>
       <c r="CC2" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="CD2" s="52" t="s">
+        <v>410</v>
+      </c>
+      <c r="CE2" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="CD2" s="52" t="s">
+      <c r="CF2" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="CE2" s="52" t="s">
+      <c r="CG2" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="CF2" s="52" t="s">
+      <c r="CH2" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="CG2" s="48"/>
+      <c r="CI2" s="48"/>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <f t="shared" ref="A3:A29" si="0">COUNTIF(D3,"&lt;&gt;"&amp;"")+COUNTIF(BR3,"&lt;&gt;"&amp;"")</f>
         <v>1</v>
@@ -3203,10 +3212,10 @@
         <v>275162</v>
       </c>
       <c r="Q3" s="54" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="S3" t="s">
         <v>49</v>
@@ -3219,10 +3228,10 @@
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="16" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="X3" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y3" s="33">
         <v>1</v>
@@ -3250,36 +3259,38 @@
         <v>49</v>
       </c>
       <c r="AH3" s="59" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AI3" s="59" t="s">
         <v>224</v>
       </c>
       <c r="AJ3" s="59" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AK3" s="59" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AL3" s="59"/>
       <c r="AM3" s="61" t="s">
         <v>195</v>
       </c>
-      <c r="AN3" s="62"/>
-      <c r="AO3" s="63">
+      <c r="AN3" s="72">
+        <v>27.8</v>
+      </c>
+      <c r="AO3" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR3" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS3" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT3" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU3" s="1" t="s">
         <v>223</v>
@@ -3315,30 +3326,30 @@
       <c r="BH3" s="57"/>
       <c r="BI3" s="57"/>
       <c r="BJ3" s="57"/>
-      <c r="BL3" s="65">
+      <c r="BL3" s="63">
         <v>41226</v>
       </c>
-      <c r="BM3" s="66" t="s">
-        <v>335</v>
-      </c>
-      <c r="BN3" s="67">
+      <c r="BM3" s="64" t="s">
+        <v>333</v>
+      </c>
+      <c r="BN3" s="65">
         <v>31.63212</v>
       </c>
-      <c r="BO3" s="67">
+      <c r="BO3" s="65">
         <v>34.5167</v>
       </c>
       <c r="BP3" s="42" t="s">
+        <v>345</v>
+      </c>
+      <c r="BQ3" t="s">
         <v>347</v>
-      </c>
-      <c r="BQ3" t="s">
-        <v>349</v>
       </c>
       <c r="BR3" s="25"/>
       <c r="BW3">
         <v>1.5</v>
       </c>
       <c r="BX3" s="42" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="BY3" s="42">
         <v>0</v>
@@ -3350,8 +3361,10 @@
       <c r="CD3"/>
       <c r="CE3"/>
       <c r="CF3"/>
+      <c r="CG3"/>
+      <c r="CH3"/>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3360,7 +3373,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>88</v>
@@ -3408,10 +3421,10 @@
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="16" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="X4" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y4" s="33">
         <v>1</v>
@@ -3439,36 +3452,36 @@
         <v>49</v>
       </c>
       <c r="AH4" s="59" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="AI4" s="59" t="s">
         <v>225</v>
       </c>
       <c r="AJ4" s="59" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="AK4" s="59" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AL4" s="59"/>
       <c r="AM4" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="AN4" s="62"/>
-      <c r="AO4" s="63">
+      <c r="AN4" s="72"/>
+      <c r="AO4" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR4" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS4" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT4" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU4" s="1" t="s">
         <v>223</v>
@@ -3504,30 +3517,30 @@
       <c r="BH4" s="57"/>
       <c r="BI4" s="57"/>
       <c r="BJ4" s="57"/>
-      <c r="BL4" s="65">
+      <c r="BL4" s="63">
         <v>41226</v>
       </c>
-      <c r="BM4" s="66" t="s">
-        <v>335</v>
-      </c>
-      <c r="BN4" s="67">
+      <c r="BM4" s="64" t="s">
+        <v>333</v>
+      </c>
+      <c r="BN4" s="65">
         <v>31.63212</v>
       </c>
-      <c r="BO4" s="67">
+      <c r="BO4" s="65">
         <v>34.5167</v>
       </c>
       <c r="BP4" s="42" t="s">
+        <v>345</v>
+      </c>
+      <c r="BQ4" t="s">
         <v>347</v>
-      </c>
-      <c r="BQ4" t="s">
-        <v>349</v>
       </c>
       <c r="BR4" s="25"/>
       <c r="BW4">
         <v>1.5</v>
       </c>
       <c r="BX4" s="42" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="BY4" s="42">
         <v>0</v>
@@ -3539,8 +3552,10 @@
       <c r="CD4"/>
       <c r="CE4"/>
       <c r="CF4"/>
+      <c r="CG4"/>
+      <c r="CH4"/>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3585,10 +3600,10 @@
         <v>367728</v>
       </c>
       <c r="Q5" s="54" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="R5" s="24" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="S5" t="s">
         <v>49</v>
@@ -3601,10 +3616,10 @@
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="16" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="X5" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y5" s="33">
         <v>1</v>
@@ -3632,36 +3647,38 @@
         <v>49</v>
       </c>
       <c r="AH5" s="59" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AI5" s="59" t="s">
         <v>226</v>
       </c>
       <c r="AJ5" s="59" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="AK5" s="59" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AL5" s="59"/>
       <c r="AM5" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="AN5" s="64"/>
-      <c r="AO5" s="63">
+      <c r="AN5" s="72">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="AO5" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR5" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS5" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT5" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU5" s="1" t="s">
         <v>223</v>
@@ -3697,30 +3714,30 @@
       <c r="BH5" s="57"/>
       <c r="BI5" s="57"/>
       <c r="BJ5" s="57"/>
-      <c r="BL5" s="65">
+      <c r="BL5" s="63">
         <v>41226</v>
       </c>
-      <c r="BM5" s="66" t="s">
-        <v>335</v>
-      </c>
-      <c r="BN5" s="67">
+      <c r="BM5" s="64" t="s">
+        <v>333</v>
+      </c>
+      <c r="BN5" s="65">
         <v>31.63212</v>
       </c>
-      <c r="BO5" s="67">
+      <c r="BO5" s="65">
         <v>34.5167</v>
       </c>
       <c r="BP5" s="42" t="s">
+        <v>345</v>
+      </c>
+      <c r="BQ5" t="s">
         <v>347</v>
-      </c>
-      <c r="BQ5" t="s">
-        <v>349</v>
       </c>
       <c r="BR5" s="25"/>
       <c r="BW5">
         <v>1.5</v>
       </c>
       <c r="BX5" s="42" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="BY5" s="42">
         <v>0</v>
@@ -3732,8 +3749,10 @@
       <c r="CD5"/>
       <c r="CE5"/>
       <c r="CF5"/>
+      <c r="CG5"/>
+      <c r="CH5"/>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3778,10 +3797,10 @@
         <v>292281</v>
       </c>
       <c r="Q6" s="55" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="R6" s="19" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="S6" t="s">
         <v>49</v>
@@ -3794,10 +3813,10 @@
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="16" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="X6" s="16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Y6" s="33">
         <v>2</v>
@@ -3825,36 +3844,38 @@
         <v>49</v>
       </c>
       <c r="AH6" s="59" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AI6" s="59" t="s">
         <v>227</v>
       </c>
       <c r="AJ6" s="59" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AK6" s="59" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AL6" s="59"/>
       <c r="AM6" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="AN6" s="62"/>
-      <c r="AO6" s="63">
+      <c r="AN6" s="72">
+        <v>42.6</v>
+      </c>
+      <c r="AO6" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR6" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS6" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT6" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU6" s="1" t="s">
         <v>223</v>
@@ -3890,32 +3911,32 @@
       <c r="BH6" s="57"/>
       <c r="BI6" s="57"/>
       <c r="BJ6" s="57"/>
-      <c r="BL6" s="65">
+      <c r="BL6" s="63">
         <v>41226</v>
       </c>
-      <c r="BM6" s="66" t="s">
-        <v>336</v>
-      </c>
-      <c r="BN6" s="67">
+      <c r="BM6" s="64" t="s">
+        <v>334</v>
+      </c>
+      <c r="BN6" s="65">
         <v>31.6341</v>
       </c>
-      <c r="BO6" s="67">
+      <c r="BO6" s="65">
         <v>34.51144</v>
       </c>
       <c r="BP6" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="BR6" s="25"/>
       <c r="BW6">
         <v>10</v>
       </c>
-      <c r="BX6" s="70" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY6" s="70">
+      <c r="BX6" s="68" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY6" s="68">
         <v>545.16</v>
       </c>
       <c r="BZ6"/>
@@ -3925,8 +3946,10 @@
       <c r="CD6"/>
       <c r="CE6"/>
       <c r="CF6"/>
+      <c r="CG6"/>
+      <c r="CH6"/>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3971,10 +3994,10 @@
         <v>242696</v>
       </c>
       <c r="Q7" s="54" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="S7" t="s">
         <v>49</v>
@@ -3987,10 +4010,10 @@
       </c>
       <c r="V7" s="1"/>
       <c r="W7" s="16" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="X7" s="16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Y7" s="33">
         <v>2</v>
@@ -4018,36 +4041,38 @@
         <v>49</v>
       </c>
       <c r="AH7" s="59" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AI7" s="59" t="s">
         <v>228</v>
       </c>
       <c r="AJ7" s="59" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AK7" s="59" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AL7" s="59"/>
       <c r="AM7" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="AN7" s="62"/>
-      <c r="AO7" s="63">
+      <c r="AN7" s="72">
+        <v>41.6</v>
+      </c>
+      <c r="AO7" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR7" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS7" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT7" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU7" s="1" t="s">
         <v>223</v>
@@ -4083,32 +4108,32 @@
       <c r="BH7" s="57"/>
       <c r="BI7" s="57"/>
       <c r="BJ7" s="57"/>
-      <c r="BL7" s="65">
+      <c r="BL7" s="63">
         <v>41226</v>
       </c>
-      <c r="BM7" s="66" t="s">
-        <v>336</v>
-      </c>
-      <c r="BN7" s="67">
+      <c r="BM7" s="64" t="s">
+        <v>334</v>
+      </c>
+      <c r="BN7" s="65">
         <v>31.6341</v>
       </c>
-      <c r="BO7" s="67">
+      <c r="BO7" s="65">
         <v>34.51144</v>
       </c>
       <c r="BP7" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="BR7" s="25"/>
       <c r="BW7">
         <v>10</v>
       </c>
-      <c r="BX7" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY7" s="71">
+      <c r="BX7" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY7" s="69">
         <v>545.16</v>
       </c>
       <c r="BZ7"/>
@@ -4118,8 +4143,10 @@
       <c r="CD7"/>
       <c r="CE7"/>
       <c r="CF7"/>
+      <c r="CG7"/>
+      <c r="CH7"/>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4164,10 +4191,10 @@
         <v>282664</v>
       </c>
       <c r="Q8" s="54" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="R8" s="24" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="S8" t="s">
         <v>49</v>
@@ -4180,10 +4207,10 @@
       </c>
       <c r="V8" s="1"/>
       <c r="W8" s="16" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="X8" s="16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Y8" s="33">
         <v>2</v>
@@ -4211,36 +4238,38 @@
         <v>49</v>
       </c>
       <c r="AH8" s="59" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AI8" s="59" t="s">
         <v>229</v>
       </c>
       <c r="AJ8" s="59" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="AK8" s="59" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="AL8" s="59"/>
       <c r="AM8" s="61" t="s">
         <v>200</v>
       </c>
-      <c r="AN8" s="62"/>
-      <c r="AO8" s="63">
+      <c r="AN8" s="72">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="AO8" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR8" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS8" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT8" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU8" s="1" t="s">
         <v>223</v>
@@ -4276,32 +4305,32 @@
       <c r="BH8" s="57"/>
       <c r="BI8" s="57"/>
       <c r="BJ8" s="57"/>
-      <c r="BL8" s="65">
+      <c r="BL8" s="63">
         <v>41226</v>
       </c>
-      <c r="BM8" s="66" t="s">
-        <v>336</v>
-      </c>
-      <c r="BN8" s="67">
+      <c r="BM8" s="64" t="s">
+        <v>334</v>
+      </c>
+      <c r="BN8" s="65">
         <v>31.6341</v>
       </c>
-      <c r="BO8" s="67">
+      <c r="BO8" s="65">
         <v>34.51144</v>
       </c>
       <c r="BP8" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ8" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="BR8" s="25"/>
       <c r="BW8">
         <v>10</v>
       </c>
-      <c r="BX8" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY8" s="71">
+      <c r="BX8" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY8" s="69">
         <v>545.16</v>
       </c>
       <c r="BZ8"/>
@@ -4311,8 +4340,10 @@
       <c r="CD8"/>
       <c r="CE8"/>
       <c r="CF8"/>
+      <c r="CG8"/>
+      <c r="CH8"/>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4357,10 +4388,10 @@
         <v>233579</v>
       </c>
       <c r="Q9" s="54" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="R9" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="S9" t="s">
         <v>49</v>
@@ -4373,10 +4404,10 @@
       </c>
       <c r="V9" s="1"/>
       <c r="W9" s="16" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="X9" s="16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Y9" s="33">
         <v>3</v>
@@ -4404,36 +4435,38 @@
         <v>49</v>
       </c>
       <c r="AH9" s="59" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="AI9" s="59" t="s">
         <v>230</v>
       </c>
       <c r="AJ9" s="59" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="AK9" s="59" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="AL9" s="59"/>
       <c r="AM9" s="61" t="s">
         <v>201</v>
       </c>
-      <c r="AN9" s="62"/>
-      <c r="AO9" s="63">
+      <c r="AN9" s="72">
+        <v>33.4</v>
+      </c>
+      <c r="AO9" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR9" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS9" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT9" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU9" s="1" t="s">
         <v>223</v>
@@ -4469,32 +4502,32 @@
       <c r="BH9" s="57"/>
       <c r="BI9" s="57"/>
       <c r="BJ9" s="57"/>
-      <c r="BL9" s="65">
+      <c r="BL9" s="63">
         <v>41226</v>
       </c>
-      <c r="BM9" s="66" t="s">
-        <v>337</v>
-      </c>
-      <c r="BN9" s="67">
+      <c r="BM9" s="64" t="s">
+        <v>335</v>
+      </c>
+      <c r="BN9" s="65">
         <v>31.671759999999999</v>
       </c>
-      <c r="BO9" s="67">
+      <c r="BO9" s="65">
         <v>34.543559999999999</v>
       </c>
       <c r="BP9" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ9" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="BR9" s="25"/>
       <c r="BW9">
         <v>5</v>
       </c>
-      <c r="BX9" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY9" s="71">
+      <c r="BX9" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY9" s="69">
         <v>5080.2700000000004</v>
       </c>
       <c r="BZ9"/>
@@ -4504,8 +4537,10 @@
       <c r="CD9"/>
       <c r="CE9"/>
       <c r="CF9"/>
+      <c r="CG9"/>
+      <c r="CH9"/>
     </row>
-    <row r="10" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4550,10 +4585,10 @@
         <v>137661</v>
       </c>
       <c r="Q10" s="54" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="S10" t="s">
         <v>49</v>
@@ -4566,10 +4601,10 @@
       </c>
       <c r="V10" s="1"/>
       <c r="W10" s="16" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="X10" s="16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Y10" s="33">
         <v>3</v>
@@ -4597,36 +4632,38 @@
         <v>49</v>
       </c>
       <c r="AH10" s="59" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AI10" s="59" t="s">
         <v>231</v>
       </c>
       <c r="AJ10" s="59" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AK10" s="59" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="AL10" s="59"/>
       <c r="AM10" s="61" t="s">
         <v>202</v>
       </c>
-      <c r="AN10" s="62"/>
-      <c r="AO10" s="63">
+      <c r="AN10" s="72">
+        <v>39</v>
+      </c>
+      <c r="AO10" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR10" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS10" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT10" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU10" s="1" t="s">
         <v>223</v>
@@ -4662,32 +4699,32 @@
       <c r="BH10" s="57"/>
       <c r="BI10" s="57"/>
       <c r="BJ10" s="57"/>
-      <c r="BL10" s="65">
+      <c r="BL10" s="63">
         <v>41226</v>
       </c>
-      <c r="BM10" s="66" t="s">
-        <v>337</v>
-      </c>
-      <c r="BN10" s="67">
+      <c r="BM10" s="64" t="s">
+        <v>335</v>
+      </c>
+      <c r="BN10" s="65">
         <v>31.671759999999999</v>
       </c>
-      <c r="BO10" s="67">
+      <c r="BO10" s="65">
         <v>34.543559999999999</v>
       </c>
       <c r="BP10" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="BR10" s="25"/>
       <c r="BW10">
         <v>5</v>
       </c>
-      <c r="BX10" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY10" s="71">
+      <c r="BX10" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY10" s="69">
         <v>5080.2700000000004</v>
       </c>
       <c r="BZ10"/>
@@ -4697,8 +4734,10 @@
       <c r="CD10"/>
       <c r="CE10"/>
       <c r="CF10"/>
+      <c r="CG10"/>
+      <c r="CH10"/>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4743,10 +4782,10 @@
         <v>273123</v>
       </c>
       <c r="Q11" s="54" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="R11" s="19" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="S11" t="s">
         <v>49</v>
@@ -4759,10 +4798,10 @@
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="16" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="X11" s="16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Y11" s="33">
         <v>3</v>
@@ -4790,36 +4829,38 @@
         <v>49</v>
       </c>
       <c r="AH11" s="59" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AI11" s="59" t="s">
         <v>232</v>
       </c>
       <c r="AJ11" s="59" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="AK11" s="59" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="AL11" s="59"/>
       <c r="AM11" s="61" t="s">
         <v>203</v>
       </c>
-      <c r="AN11" s="62"/>
-      <c r="AO11" s="63">
+      <c r="AN11" s="72">
+        <v>27.6</v>
+      </c>
+      <c r="AO11" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR11" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS11" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT11" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU11" s="1" t="s">
         <v>223</v>
@@ -4855,32 +4896,32 @@
       <c r="BH11" s="57"/>
       <c r="BI11" s="57"/>
       <c r="BJ11" s="57"/>
-      <c r="BL11" s="65">
+      <c r="BL11" s="63">
         <v>41226</v>
       </c>
-      <c r="BM11" s="66" t="s">
-        <v>337</v>
-      </c>
-      <c r="BN11" s="67">
+      <c r="BM11" s="64" t="s">
+        <v>335</v>
+      </c>
+      <c r="BN11" s="65">
         <v>31.671759999999999</v>
       </c>
-      <c r="BO11" s="67">
+      <c r="BO11" s="65">
         <v>34.543559999999999</v>
       </c>
       <c r="BP11" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ11" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="BR11" s="25"/>
       <c r="BW11">
         <v>5</v>
       </c>
-      <c r="BX11" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY11" s="71">
+      <c r="BX11" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY11" s="69">
         <v>5080.2700000000004</v>
       </c>
       <c r="BZ11"/>
@@ -4890,8 +4931,10 @@
       <c r="CD11"/>
       <c r="CE11"/>
       <c r="CF11"/>
+      <c r="CG11"/>
+      <c r="CH11"/>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4936,10 +4979,10 @@
         <v>134807</v>
       </c>
       <c r="Q12" s="54" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="R12" s="24" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="S12" t="s">
         <v>49</v>
@@ -4952,10 +4995,10 @@
       </c>
       <c r="V12" s="1"/>
       <c r="W12" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="X12" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y12" s="33">
         <v>4</v>
@@ -4983,36 +5026,38 @@
         <v>49</v>
       </c>
       <c r="AH12" s="59" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="AI12" s="59" t="s">
         <v>233</v>
       </c>
       <c r="AJ12" s="59" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="AK12" s="59" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="AL12" s="59"/>
       <c r="AM12" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="AN12" s="62"/>
-      <c r="AO12" s="63">
+      <c r="AN12" s="72">
+        <v>32</v>
+      </c>
+      <c r="AO12" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR12" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS12" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT12" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU12" s="1" t="s">
         <v>223</v>
@@ -5048,30 +5093,30 @@
       <c r="BH12" s="57"/>
       <c r="BI12" s="57"/>
       <c r="BJ12" s="57"/>
-      <c r="BL12" s="65">
+      <c r="BL12" s="63">
         <v>41227</v>
       </c>
-      <c r="BM12" s="66" t="s">
-        <v>338</v>
-      </c>
-      <c r="BN12" s="67">
+      <c r="BM12" s="64" t="s">
+        <v>336</v>
+      </c>
+      <c r="BN12" s="65">
         <v>31.941859999999998</v>
       </c>
-      <c r="BO12" s="67">
+      <c r="BO12" s="65">
         <v>34.68862</v>
       </c>
       <c r="BP12" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ12" s="58" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="BR12" s="25"/>
       <c r="BW12">
         <v>18</v>
       </c>
-      <c r="BX12" s="71" t="s">
-        <v>346</v>
+      <c r="BX12" s="69" t="s">
+        <v>344</v>
       </c>
       <c r="BY12" s="42">
         <v>0</v>
@@ -5083,8 +5128,10 @@
       <c r="CD12"/>
       <c r="CE12"/>
       <c r="CF12"/>
+      <c r="CG12"/>
+      <c r="CH12"/>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5129,10 +5176,10 @@
         <v>244784</v>
       </c>
       <c r="Q13" s="54" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="R13" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="S13" t="s">
         <v>49</v>
@@ -5145,10 +5192,10 @@
       </c>
       <c r="V13" s="1"/>
       <c r="W13" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="X13" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y13" s="33">
         <v>4</v>
@@ -5176,36 +5223,38 @@
         <v>49</v>
       </c>
       <c r="AH13" s="59" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AI13" s="59" t="s">
         <v>234</v>
       </c>
       <c r="AJ13" s="59" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="AK13" s="59" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="AL13" s="59"/>
       <c r="AM13" s="61" t="s">
         <v>205</v>
       </c>
-      <c r="AN13" s="62"/>
-      <c r="AO13" s="63">
+      <c r="AN13" s="72">
+        <v>45.6</v>
+      </c>
+      <c r="AO13" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR13" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS13" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT13" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU13" s="1" t="s">
         <v>223</v>
@@ -5241,30 +5290,30 @@
       <c r="BH13" s="57"/>
       <c r="BI13" s="57"/>
       <c r="BJ13" s="57"/>
-      <c r="BL13" s="65">
+      <c r="BL13" s="63">
         <v>41227</v>
       </c>
-      <c r="BM13" s="66" t="s">
-        <v>338</v>
-      </c>
-      <c r="BN13" s="67">
+      <c r="BM13" s="64" t="s">
+        <v>336</v>
+      </c>
+      <c r="BN13" s="65">
         <v>31.941859999999998</v>
       </c>
-      <c r="BO13" s="67">
+      <c r="BO13" s="65">
         <v>34.68862</v>
       </c>
       <c r="BP13" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ13" s="58" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="BR13" s="25"/>
       <c r="BW13">
         <v>18</v>
       </c>
-      <c r="BX13" s="71" t="s">
-        <v>346</v>
+      <c r="BX13" s="69" t="s">
+        <v>344</v>
       </c>
       <c r="BY13" s="42">
         <v>0</v>
@@ -5276,8 +5325,10 @@
       <c r="CD13"/>
       <c r="CE13"/>
       <c r="CF13"/>
+      <c r="CG13"/>
+      <c r="CH13"/>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5322,10 +5373,10 @@
         <v>337801</v>
       </c>
       <c r="Q14" s="55" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="R14" s="19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="S14" t="s">
         <v>49</v>
@@ -5338,10 +5389,10 @@
       </c>
       <c r="V14" s="1"/>
       <c r="W14" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="X14" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y14" s="33">
         <v>4</v>
@@ -5369,36 +5420,38 @@
         <v>49</v>
       </c>
       <c r="AH14" s="59" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="AI14" s="59" t="s">
         <v>235</v>
       </c>
       <c r="AJ14" s="59" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AK14" s="59" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AL14" s="59"/>
       <c r="AM14" s="61" t="s">
         <v>206</v>
       </c>
-      <c r="AN14" s="62"/>
-      <c r="AO14" s="63">
+      <c r="AN14" s="72">
+        <v>30</v>
+      </c>
+      <c r="AO14" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR14" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS14" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT14" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU14" s="1" t="s">
         <v>223</v>
@@ -5434,30 +5487,30 @@
       <c r="BH14" s="57"/>
       <c r="BI14" s="57"/>
       <c r="BJ14" s="57"/>
-      <c r="BL14" s="65">
+      <c r="BL14" s="63">
         <v>41227</v>
       </c>
-      <c r="BM14" s="66" t="s">
-        <v>338</v>
-      </c>
-      <c r="BN14" s="67">
+      <c r="BM14" s="64" t="s">
+        <v>336</v>
+      </c>
+      <c r="BN14" s="65">
         <v>31.941859999999998</v>
       </c>
-      <c r="BO14" s="67">
+      <c r="BO14" s="65">
         <v>34.68862</v>
       </c>
       <c r="BP14" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ14" s="58" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="BR14" s="25"/>
       <c r="BW14">
         <v>18</v>
       </c>
-      <c r="BX14" s="71" t="s">
-        <v>346</v>
+      <c r="BX14" s="69" t="s">
+        <v>344</v>
       </c>
       <c r="BY14" s="42">
         <v>0</v>
@@ -5469,8 +5522,10 @@
       <c r="CD14"/>
       <c r="CE14"/>
       <c r="CF14"/>
+      <c r="CG14"/>
+      <c r="CH14"/>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5515,10 +5570,10 @@
         <v>252074</v>
       </c>
       <c r="Q15" s="54" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="R15" s="19" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="S15" t="s">
         <v>49</v>
@@ -5531,10 +5586,10 @@
       </c>
       <c r="V15" s="1"/>
       <c r="W15" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="X15" s="16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Y15" s="33">
         <v>5</v>
@@ -5562,36 +5617,38 @@
         <v>49</v>
       </c>
       <c r="AH15" s="59" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="AI15" s="59" t="s">
         <v>236</v>
       </c>
       <c r="AJ15" s="59" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AK15" s="59" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AL15" s="59"/>
       <c r="AM15" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="AN15" s="62"/>
-      <c r="AO15" s="63">
+      <c r="AN15" s="72">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="AO15" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR15" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS15" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT15" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU15" s="1" t="s">
         <v>223</v>
@@ -5627,32 +5684,32 @@
       <c r="BH15" s="57"/>
       <c r="BI15" s="57"/>
       <c r="BJ15" s="57"/>
-      <c r="BL15" s="65">
+      <c r="BL15" s="63">
         <v>41227</v>
       </c>
-      <c r="BM15" s="66" t="s">
-        <v>339</v>
-      </c>
-      <c r="BN15" s="67">
+      <c r="BM15" s="64" t="s">
+        <v>337</v>
+      </c>
+      <c r="BN15" s="65">
         <v>31.94068</v>
       </c>
-      <c r="BO15" s="67">
+      <c r="BO15" s="65">
         <v>34.687379999999997</v>
       </c>
       <c r="BP15" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ15" s="58" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="BR15" s="25"/>
       <c r="BW15">
         <v>19</v>
       </c>
-      <c r="BX15" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY15" s="70">
+      <c r="BX15" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY15" s="68">
         <v>175.69</v>
       </c>
       <c r="BZ15"/>
@@ -5662,8 +5719,10 @@
       <c r="CD15"/>
       <c r="CE15"/>
       <c r="CF15"/>
+      <c r="CG15"/>
+      <c r="CH15"/>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5706,10 +5765,10 @@
         <v>154501</v>
       </c>
       <c r="Q16" s="54" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="R16" s="19" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="S16" t="s">
         <v>49</v>
@@ -5722,10 +5781,10 @@
       </c>
       <c r="V16" s="1"/>
       <c r="W16" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="X16" s="16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Y16" s="33">
         <v>5</v>
@@ -5751,36 +5810,38 @@
       </c>
       <c r="AG16" s="1"/>
       <c r="AH16" s="59" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="AI16" s="59" t="s">
         <v>237</v>
       </c>
       <c r="AJ16" s="59" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AK16" s="59" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="AL16" s="59"/>
       <c r="AM16" s="61" t="s">
         <v>208</v>
       </c>
-      <c r="AN16" s="62"/>
-      <c r="AO16" s="63">
+      <c r="AN16" s="72">
+        <v>34.4</v>
+      </c>
+      <c r="AO16" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ16" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR16" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS16" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT16" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU16" s="1" t="s">
         <v>223</v>
@@ -5813,32 +5874,32 @@
       <c r="BH16" s="57"/>
       <c r="BI16" s="57"/>
       <c r="BJ16" s="57"/>
-      <c r="BL16" s="65">
+      <c r="BL16" s="63">
         <v>41227</v>
       </c>
-      <c r="BM16" s="66" t="s">
-        <v>339</v>
-      </c>
-      <c r="BN16" s="67">
+      <c r="BM16" s="64" t="s">
+        <v>337</v>
+      </c>
+      <c r="BN16" s="65">
         <v>31.94068</v>
       </c>
-      <c r="BO16" s="67">
+      <c r="BO16" s="65">
         <v>34.687379999999997</v>
       </c>
       <c r="BP16" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ16" s="58" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="BR16" s="25"/>
       <c r="BW16">
         <v>19</v>
       </c>
-      <c r="BX16" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY16" s="71">
+      <c r="BX16" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY16" s="69">
         <v>175.69</v>
       </c>
       <c r="BZ16"/>
@@ -5848,8 +5909,10 @@
       <c r="CD16"/>
       <c r="CE16"/>
       <c r="CF16"/>
+      <c r="CG16"/>
+      <c r="CH16"/>
     </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5892,10 +5955,10 @@
         <v>174238</v>
       </c>
       <c r="Q17" s="55" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="R17" s="19" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="S17" t="s">
         <v>49</v>
@@ -5908,10 +5971,10 @@
       </c>
       <c r="V17" s="1"/>
       <c r="W17" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="X17" s="16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Y17" s="33">
         <v>5</v>
@@ -5937,36 +6000,38 @@
       </c>
       <c r="AG17" s="1"/>
       <c r="AH17" s="59" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AI17" s="59" t="s">
         <v>238</v>
       </c>
       <c r="AJ17" s="59" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AK17" s="59" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AL17" s="59"/>
       <c r="AM17" s="61" t="s">
         <v>209</v>
       </c>
-      <c r="AN17" s="62"/>
-      <c r="AO17" s="63">
+      <c r="AN17" s="72">
+        <v>35.6</v>
+      </c>
+      <c r="AO17" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ17" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR17" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS17" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT17" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU17" s="1" t="s">
         <v>223</v>
@@ -5999,32 +6064,32 @@
       <c r="BH17" s="57"/>
       <c r="BI17" s="57"/>
       <c r="BJ17" s="57"/>
-      <c r="BL17" s="65">
+      <c r="BL17" s="63">
         <v>41227</v>
       </c>
-      <c r="BM17" s="66" t="s">
-        <v>339</v>
-      </c>
-      <c r="BN17" s="67">
+      <c r="BM17" s="64" t="s">
+        <v>337</v>
+      </c>
+      <c r="BN17" s="65">
         <v>31.94068</v>
       </c>
-      <c r="BO17" s="67">
+      <c r="BO17" s="65">
         <v>34.687379999999997</v>
       </c>
       <c r="BP17" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ17" s="58" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="BR17" s="25"/>
       <c r="BW17">
         <v>19</v>
       </c>
-      <c r="BX17" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY17" s="71">
+      <c r="BX17" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY17" s="69">
         <v>175.69</v>
       </c>
       <c r="BZ17"/>
@@ -6034,8 +6099,10 @@
       <c r="CD17"/>
       <c r="CE17"/>
       <c r="CF17"/>
+      <c r="CG17"/>
+      <c r="CH17"/>
     </row>
-    <row r="18" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6078,10 +6145,10 @@
         <v>171763</v>
       </c>
       <c r="Q18" s="54" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="R18" s="19" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="S18" t="s">
         <v>49</v>
@@ -6094,10 +6161,10 @@
       </c>
       <c r="V18" s="1"/>
       <c r="W18" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="X18" s="16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Y18" s="33">
         <v>6</v>
@@ -6123,36 +6190,38 @@
       </c>
       <c r="AG18" s="1"/>
       <c r="AH18" s="59" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="AI18" s="59" t="s">
         <v>239</v>
       </c>
       <c r="AJ18" s="59" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AK18" s="59" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AL18" s="59"/>
       <c r="AM18" s="61" t="s">
         <v>210</v>
       </c>
-      <c r="AN18" s="62"/>
-      <c r="AO18" s="63">
+      <c r="AN18" s="72">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="AO18" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR18" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS18" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT18" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU18" s="1" t="s">
         <v>223</v>
@@ -6185,32 +6254,32 @@
       <c r="BH18" s="57"/>
       <c r="BI18" s="57"/>
       <c r="BJ18" s="57"/>
-      <c r="BL18" s="65">
+      <c r="BL18" s="63">
         <v>41227</v>
       </c>
-      <c r="BM18" s="66" t="s">
-        <v>340</v>
-      </c>
-      <c r="BN18" s="67">
+      <c r="BM18" s="64" t="s">
+        <v>338</v>
+      </c>
+      <c r="BN18" s="65">
         <v>31.931660000000001</v>
       </c>
-      <c r="BO18" s="67">
+      <c r="BO18" s="65">
         <v>34.68336</v>
       </c>
       <c r="BP18" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ18" s="58" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="BR18" s="25"/>
       <c r="BW18">
         <v>18</v>
       </c>
-      <c r="BX18" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY18" s="71">
+      <c r="BX18" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY18" s="69">
         <v>1235.56</v>
       </c>
       <c r="BZ18"/>
@@ -6220,8 +6289,10 @@
       <c r="CD18"/>
       <c r="CE18"/>
       <c r="CF18"/>
+      <c r="CG18"/>
+      <c r="CH18"/>
     </row>
-    <row r="19" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6264,10 +6335,10 @@
         <v>237422</v>
       </c>
       <c r="Q19" s="54" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="R19" s="19" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="S19" t="s">
         <v>49</v>
@@ -6280,10 +6351,10 @@
       </c>
       <c r="V19" s="1"/>
       <c r="W19" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="X19" s="16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Y19" s="33">
         <v>6</v>
@@ -6309,36 +6380,38 @@
       </c>
       <c r="AG19" s="1"/>
       <c r="AH19" s="59" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AI19" s="59" t="s">
         <v>240</v>
       </c>
       <c r="AJ19" s="59" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AK19" s="59" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AL19" s="59"/>
       <c r="AM19" s="61" t="s">
         <v>211</v>
       </c>
-      <c r="AN19" s="62"/>
-      <c r="AO19" s="63">
+      <c r="AN19" s="72">
+        <v>34.6</v>
+      </c>
+      <c r="AO19" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR19" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS19" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT19" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU19" s="1" t="s">
         <v>223</v>
@@ -6371,32 +6444,32 @@
       <c r="BH19" s="57"/>
       <c r="BI19" s="57"/>
       <c r="BJ19" s="57"/>
-      <c r="BL19" s="65">
+      <c r="BL19" s="63">
         <v>41227</v>
       </c>
-      <c r="BM19" s="66" t="s">
-        <v>340</v>
-      </c>
-      <c r="BN19" s="67">
+      <c r="BM19" s="64" t="s">
+        <v>338</v>
+      </c>
+      <c r="BN19" s="65">
         <v>31.931660000000001</v>
       </c>
-      <c r="BO19" s="67">
+      <c r="BO19" s="65">
         <v>34.68336</v>
       </c>
       <c r="BP19" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ19" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="BR19" s="25"/>
       <c r="BW19">
         <v>18</v>
       </c>
-      <c r="BX19" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY19" s="71">
+      <c r="BX19" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY19" s="69">
         <v>1235.56</v>
       </c>
       <c r="BZ19"/>
@@ -6406,8 +6479,10 @@
       <c r="CD19"/>
       <c r="CE19"/>
       <c r="CF19"/>
+      <c r="CG19"/>
+      <c r="CH19"/>
     </row>
-    <row r="20" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6450,10 +6525,10 @@
         <v>154346</v>
       </c>
       <c r="Q20" s="54" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="R20" s="19" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="S20" t="s">
         <v>49</v>
@@ -6466,10 +6541,10 @@
       </c>
       <c r="V20" s="1"/>
       <c r="W20" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="X20" s="16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Y20" s="33">
         <v>6</v>
@@ -6495,36 +6570,38 @@
       </c>
       <c r="AG20" s="1"/>
       <c r="AH20" s="59" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="AI20" s="59" t="s">
         <v>241</v>
       </c>
       <c r="AJ20" s="59" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="AK20" s="59" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="AL20" s="59"/>
       <c r="AM20" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="AN20" s="62"/>
-      <c r="AO20" s="63">
+      <c r="AN20" s="72">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="AO20" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR20" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS20" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT20" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU20" s="1" t="s">
         <v>223</v>
@@ -6557,32 +6634,32 @@
       <c r="BH20" s="57"/>
       <c r="BI20" s="57"/>
       <c r="BJ20" s="57"/>
-      <c r="BL20" s="65">
+      <c r="BL20" s="63">
         <v>41227</v>
       </c>
-      <c r="BM20" s="66" t="s">
-        <v>340</v>
-      </c>
-      <c r="BN20" s="67">
+      <c r="BM20" s="64" t="s">
+        <v>338</v>
+      </c>
+      <c r="BN20" s="65">
         <v>31.931660000000001</v>
       </c>
-      <c r="BO20" s="67">
+      <c r="BO20" s="65">
         <v>34.68336</v>
       </c>
       <c r="BP20" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ20" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="BR20" s="25"/>
       <c r="BW20">
         <v>18</v>
       </c>
-      <c r="BX20" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY20" s="71">
+      <c r="BX20" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY20" s="69">
         <v>1235.56</v>
       </c>
       <c r="BZ20"/>
@@ -6592,8 +6669,10 @@
       <c r="CD20"/>
       <c r="CE20"/>
       <c r="CF20"/>
+      <c r="CG20"/>
+      <c r="CH20"/>
     </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6602,7 +6681,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="60" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D21" s="27" t="s">
         <v>105</v>
@@ -6648,10 +6727,10 @@
       </c>
       <c r="V21" s="1"/>
       <c r="W21" s="16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="X21" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y21" s="33">
         <v>7</v>
@@ -6677,36 +6756,36 @@
       </c>
       <c r="AG21" s="1"/>
       <c r="AH21" s="59" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AI21" s="59" t="s">
         <v>242</v>
       </c>
       <c r="AJ21" s="59" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AK21" s="59" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AL21" s="59"/>
       <c r="AM21" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="AN21" s="62"/>
-      <c r="AO21" s="63">
+      <c r="AN21" s="72"/>
+      <c r="AO21" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ21" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR21" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS21" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT21" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU21" s="1" t="s">
         <v>223</v>
@@ -6739,30 +6818,30 @@
       <c r="BH21" s="57"/>
       <c r="BI21" s="57"/>
       <c r="BJ21" s="57"/>
-      <c r="BL21" s="65">
+      <c r="BL21" s="63">
         <v>41233</v>
       </c>
-      <c r="BM21" s="66" t="s">
-        <v>341</v>
-      </c>
-      <c r="BN21" s="67">
+      <c r="BM21" s="64" t="s">
+        <v>339</v>
+      </c>
+      <c r="BN21" s="65">
         <v>32.465020000000003</v>
       </c>
-      <c r="BO21" s="67">
+      <c r="BO21" s="65">
         <v>34.882582999999997</v>
       </c>
       <c r="BP21" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ21" s="58" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="BR21" s="25"/>
       <c r="BW21">
         <v>3.8</v>
       </c>
       <c r="BX21" s="42" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="BY21" s="42">
         <v>0</v>
@@ -6774,8 +6853,10 @@
       <c r="CD21"/>
       <c r="CE21"/>
       <c r="CF21"/>
+      <c r="CG21"/>
+      <c r="CH21"/>
     </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6818,10 +6899,10 @@
         <v>356730</v>
       </c>
       <c r="Q22" s="54" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="R22" s="19" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="S22" t="s">
         <v>49</v>
@@ -6834,10 +6915,10 @@
       </c>
       <c r="V22" s="1"/>
       <c r="W22" s="16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="X22" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y22" s="33">
         <v>7</v>
@@ -6863,36 +6944,38 @@
       </c>
       <c r="AG22" s="1"/>
       <c r="AH22" s="59" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AI22" s="59" t="s">
         <v>243</v>
       </c>
       <c r="AJ22" s="59" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AK22" s="59" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="AL22" s="59"/>
       <c r="AM22" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="AN22" s="62"/>
-      <c r="AO22" s="63">
+      <c r="AN22" s="72">
+        <v>29.4</v>
+      </c>
+      <c r="AO22" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR22" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS22" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT22" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU22" s="1" t="s">
         <v>223</v>
@@ -6925,30 +7008,30 @@
       <c r="BH22" s="57"/>
       <c r="BI22" s="57"/>
       <c r="BJ22" s="57"/>
-      <c r="BL22" s="65">
+      <c r="BL22" s="63">
         <v>41233</v>
       </c>
-      <c r="BM22" s="66" t="s">
-        <v>341</v>
-      </c>
-      <c r="BN22" s="67">
+      <c r="BM22" s="64" t="s">
+        <v>339</v>
+      </c>
+      <c r="BN22" s="65">
         <v>32.465020000000003</v>
       </c>
-      <c r="BO22" s="67">
+      <c r="BO22" s="65">
         <v>34.882582999999997</v>
       </c>
       <c r="BP22" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ22" s="58" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="BR22" s="25"/>
       <c r="BW22">
         <v>3.8</v>
       </c>
       <c r="BX22" s="42" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="BY22" s="42">
         <v>0</v>
@@ -6960,8 +7043,10 @@
       <c r="CD22"/>
       <c r="CE22"/>
       <c r="CF22"/>
+      <c r="CG22"/>
+      <c r="CH22"/>
     </row>
-    <row r="23" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7004,10 +7089,10 @@
         <v>406279</v>
       </c>
       <c r="Q23" s="54" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="R23" s="19" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="S23" t="s">
         <v>49</v>
@@ -7020,10 +7105,10 @@
       </c>
       <c r="V23" s="1"/>
       <c r="W23" s="16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="X23" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y23" s="33">
         <v>7</v>
@@ -7049,36 +7134,38 @@
       </c>
       <c r="AG23" s="1"/>
       <c r="AH23" s="59" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AI23" s="59" t="s">
         <v>244</v>
       </c>
       <c r="AJ23" s="59" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AK23" s="59" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AL23" s="59"/>
       <c r="AM23" s="61" t="s">
         <v>215</v>
       </c>
-      <c r="AN23" s="62"/>
-      <c r="AO23" s="63">
+      <c r="AN23" s="72">
+        <v>20.2</v>
+      </c>
+      <c r="AO23" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ23" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR23" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS23" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT23" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU23" s="1" t="s">
         <v>223</v>
@@ -7111,30 +7198,30 @@
       <c r="BH23" s="57"/>
       <c r="BI23" s="57"/>
       <c r="BJ23" s="57"/>
-      <c r="BL23" s="65">
+      <c r="BL23" s="63">
         <v>41233</v>
       </c>
-      <c r="BM23" s="66" t="s">
-        <v>341</v>
-      </c>
-      <c r="BN23" s="67">
+      <c r="BM23" s="64" t="s">
+        <v>339</v>
+      </c>
+      <c r="BN23" s="65">
         <v>32.465020000000003</v>
       </c>
-      <c r="BO23" s="67">
+      <c r="BO23" s="65">
         <v>34.882582999999997</v>
       </c>
       <c r="BP23" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ23" s="58" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="BR23" s="25"/>
       <c r="BW23">
         <v>3.8</v>
       </c>
       <c r="BX23" s="42" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="BY23" s="42">
         <v>0</v>
@@ -7146,8 +7233,10 @@
       <c r="CD23"/>
       <c r="CE23"/>
       <c r="CF23"/>
+      <c r="CG23"/>
+      <c r="CH23"/>
     </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7190,10 +7279,10 @@
         <v>292338</v>
       </c>
       <c r="Q24" s="54" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="R24" s="19" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="S24" t="s">
         <v>49</v>
@@ -7206,10 +7295,10 @@
       </c>
       <c r="V24" s="1"/>
       <c r="W24" s="16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="X24" s="16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Y24" s="33">
         <v>8</v>
@@ -7235,36 +7324,38 @@
       </c>
       <c r="AG24" s="1"/>
       <c r="AH24" s="59" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AI24" s="59" t="s">
         <v>245</v>
       </c>
       <c r="AJ24" s="59" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AK24" s="59" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AL24" s="59"/>
       <c r="AM24" s="61" t="s">
         <v>216</v>
       </c>
-      <c r="AN24" s="62"/>
-      <c r="AO24" s="63">
+      <c r="AN24" s="72">
+        <v>43.6</v>
+      </c>
+      <c r="AO24" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR24" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS24" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT24" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU24" s="1" t="s">
         <v>223</v>
@@ -7297,32 +7388,32 @@
       <c r="BH24" s="57"/>
       <c r="BI24" s="57"/>
       <c r="BJ24" s="57"/>
-      <c r="BL24" s="65">
+      <c r="BL24" s="63">
         <v>41233</v>
       </c>
-      <c r="BM24" s="66" t="s">
-        <v>342</v>
-      </c>
-      <c r="BN24" s="67">
+      <c r="BM24" s="64" t="s">
+        <v>340</v>
+      </c>
+      <c r="BN24" s="65">
         <v>32.463700000000003</v>
       </c>
-      <c r="BO24" s="67">
+      <c r="BO24" s="65">
         <v>34.879339999999999</v>
       </c>
       <c r="BP24" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ24" s="58" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="BR24" s="25"/>
       <c r="BW24">
         <v>5.5</v>
       </c>
-      <c r="BX24" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY24" s="70">
+      <c r="BX24" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY24" s="68">
         <v>338.21</v>
       </c>
       <c r="BZ24"/>
@@ -7332,8 +7423,10 @@
       <c r="CD24"/>
       <c r="CE24"/>
       <c r="CF24"/>
+      <c r="CG24"/>
+      <c r="CH24"/>
     </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7376,10 +7469,10 @@
         <v>269103</v>
       </c>
       <c r="Q25" s="54" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="R25" s="19" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="S25" t="s">
         <v>49</v>
@@ -7392,10 +7485,10 @@
       </c>
       <c r="V25" s="1"/>
       <c r="W25" s="16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="X25" s="16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Y25" s="33">
         <v>8</v>
@@ -7421,36 +7514,38 @@
       </c>
       <c r="AG25" s="1"/>
       <c r="AH25" s="59" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AI25" s="59" t="s">
         <v>246</v>
       </c>
       <c r="AJ25" s="59" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="AK25" s="59" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AL25" s="59"/>
       <c r="AM25" s="61" t="s">
         <v>217</v>
       </c>
-      <c r="AN25" s="62"/>
-      <c r="AO25" s="63">
+      <c r="AN25" s="72">
+        <v>15.9</v>
+      </c>
+      <c r="AO25" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ25" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR25" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS25" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT25" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU25" s="1" t="s">
         <v>223</v>
@@ -7483,32 +7578,32 @@
       <c r="BH25" s="57"/>
       <c r="BI25" s="57"/>
       <c r="BJ25" s="57"/>
-      <c r="BL25" s="65">
+      <c r="BL25" s="63">
         <v>41233</v>
       </c>
-      <c r="BM25" s="66" t="s">
-        <v>342</v>
-      </c>
-      <c r="BN25" s="67">
+      <c r="BM25" s="64" t="s">
+        <v>340</v>
+      </c>
+      <c r="BN25" s="65">
         <v>32.463700000000003</v>
       </c>
-      <c r="BO25" s="67">
+      <c r="BO25" s="65">
         <v>34.879339999999999</v>
       </c>
       <c r="BP25" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ25" s="58" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="BR25" s="25"/>
       <c r="BW25">
         <v>5.5</v>
       </c>
-      <c r="BX25" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY25" s="71">
+      <c r="BX25" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY25" s="69">
         <v>338.21</v>
       </c>
       <c r="BZ25"/>
@@ -7518,8 +7613,10 @@
       <c r="CD25"/>
       <c r="CE25"/>
       <c r="CF25"/>
+      <c r="CG25"/>
+      <c r="CH25"/>
     </row>
-    <row r="26" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7528,7 +7625,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="60" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D26" s="27" t="s">
         <v>110</v>
@@ -7574,10 +7671,10 @@
       </c>
       <c r="V26" s="1"/>
       <c r="W26" s="16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="X26" s="16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Y26" s="33">
         <v>8</v>
@@ -7603,36 +7700,36 @@
       </c>
       <c r="AG26" s="1"/>
       <c r="AH26" s="59" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AI26" s="59" t="s">
         <v>247</v>
       </c>
       <c r="AJ26" s="59" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AK26" s="59" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AL26" s="59"/>
       <c r="AM26" s="61" t="s">
         <v>218</v>
       </c>
-      <c r="AN26" s="62"/>
-      <c r="AO26" s="63">
+      <c r="AN26" s="72"/>
+      <c r="AO26" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ26" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR26" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS26" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT26" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU26" s="1" t="s">
         <v>223</v>
@@ -7665,32 +7762,32 @@
       <c r="BH26" s="57"/>
       <c r="BI26" s="57"/>
       <c r="BJ26" s="57"/>
-      <c r="BL26" s="65">
+      <c r="BL26" s="63">
         <v>41233</v>
       </c>
-      <c r="BM26" s="66" t="s">
-        <v>342</v>
-      </c>
-      <c r="BN26" s="67">
+      <c r="BM26" s="64" t="s">
+        <v>340</v>
+      </c>
+      <c r="BN26" s="65">
         <v>32.463700000000003</v>
       </c>
-      <c r="BO26" s="67">
+      <c r="BO26" s="65">
         <v>34.879339999999999</v>
       </c>
       <c r="BP26" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ26" s="58" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="BR26" s="25"/>
       <c r="BW26">
         <v>5.5</v>
       </c>
-      <c r="BX26" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY26" s="71">
+      <c r="BX26" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY26" s="69">
         <v>338.21</v>
       </c>
       <c r="BZ26"/>
@@ -7700,8 +7797,10 @@
       <c r="CD26"/>
       <c r="CE26"/>
       <c r="CF26"/>
+      <c r="CG26"/>
+      <c r="CH26"/>
     </row>
-    <row r="27" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7744,10 +7843,10 @@
         <v>190462</v>
       </c>
       <c r="Q27" s="54" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="R27" s="19" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="S27" t="s">
         <v>49</v>
@@ -7760,10 +7859,10 @@
       </c>
       <c r="V27" s="1"/>
       <c r="W27" s="16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="X27" s="16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Y27" s="33">
         <v>9</v>
@@ -7789,36 +7888,38 @@
       </c>
       <c r="AG27" s="1"/>
       <c r="AH27" s="59" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AI27" s="59" t="s">
         <v>248</v>
       </c>
       <c r="AJ27" s="59" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AK27" s="59" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AL27" s="59"/>
       <c r="AM27" s="61" t="s">
         <v>219</v>
       </c>
-      <c r="AN27" s="62"/>
-      <c r="AO27" s="63">
+      <c r="AN27" s="72">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="AO27" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ27" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR27" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS27" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT27" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU27" s="1" t="s">
         <v>223</v>
@@ -7851,32 +7952,32 @@
       <c r="BH27" s="57"/>
       <c r="BI27" s="57"/>
       <c r="BJ27" s="57"/>
-      <c r="BL27" s="65">
+      <c r="BL27" s="63">
         <v>41233</v>
       </c>
-      <c r="BM27" s="66" t="s">
-        <v>343</v>
-      </c>
-      <c r="BN27" s="67">
+      <c r="BM27" s="64" t="s">
+        <v>341</v>
+      </c>
+      <c r="BN27" s="65">
         <v>32.42868</v>
       </c>
-      <c r="BO27" s="67">
+      <c r="BO27" s="65">
         <v>34.870280000000001</v>
       </c>
       <c r="BP27" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ27" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="BR27" s="25"/>
       <c r="BW27">
         <v>6.5</v>
       </c>
-      <c r="BX27" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY27" s="71">
+      <c r="BX27" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY27" s="69">
         <v>4192.68</v>
       </c>
       <c r="BZ27"/>
@@ -7886,8 +7987,10 @@
       <c r="CD27"/>
       <c r="CE27"/>
       <c r="CF27"/>
+      <c r="CG27"/>
+      <c r="CH27"/>
     </row>
-    <row r="28" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7896,7 +7999,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="60" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D28" s="27" t="s">
         <v>112</v>
@@ -7942,10 +8045,10 @@
       </c>
       <c r="V28" s="1"/>
       <c r="W28" s="16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="X28" s="16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Y28" s="33">
         <v>9</v>
@@ -7971,36 +8074,36 @@
       </c>
       <c r="AG28" s="1"/>
       <c r="AH28" s="59" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AI28" s="59" t="s">
         <v>249</v>
       </c>
       <c r="AJ28" s="59" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AK28" s="59" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AL28" s="59"/>
       <c r="AM28" s="61" t="s">
         <v>220</v>
       </c>
-      <c r="AN28" s="62"/>
-      <c r="AO28" s="63">
+      <c r="AN28" s="72"/>
+      <c r="AO28" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ28" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR28" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS28" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT28" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU28" s="1" t="s">
         <v>223</v>
@@ -8033,32 +8136,32 @@
       <c r="BH28" s="57"/>
       <c r="BI28" s="57"/>
       <c r="BJ28" s="57"/>
-      <c r="BL28" s="65">
+      <c r="BL28" s="63">
         <v>41233</v>
       </c>
-      <c r="BM28" s="66" t="s">
-        <v>343</v>
-      </c>
-      <c r="BN28" s="67">
+      <c r="BM28" s="64" t="s">
+        <v>341</v>
+      </c>
+      <c r="BN28" s="65">
         <v>32.42868</v>
       </c>
-      <c r="BO28" s="67">
+      <c r="BO28" s="65">
         <v>34.870280000000001</v>
       </c>
       <c r="BP28" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ28" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="BR28" s="25"/>
       <c r="BW28">
         <v>6.5</v>
       </c>
-      <c r="BX28" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY28" s="71">
+      <c r="BX28" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY28" s="69">
         <v>4192.68</v>
       </c>
       <c r="BZ28"/>
@@ -8068,8 +8171,10 @@
       <c r="CD28"/>
       <c r="CE28"/>
       <c r="CF28"/>
+      <c r="CG28"/>
+      <c r="CH28"/>
     </row>
-    <row r="29" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -8078,7 +8183,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="60" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D29" s="27" t="s">
         <v>113</v>
@@ -8124,10 +8229,10 @@
       </c>
       <c r="V29" s="1"/>
       <c r="W29" s="16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="X29" s="16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Y29" s="33">
         <v>9</v>
@@ -8153,36 +8258,36 @@
       </c>
       <c r="AG29" s="1"/>
       <c r="AH29" s="59" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AI29" s="59" t="s">
         <v>224</v>
       </c>
       <c r="AJ29" s="59" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AK29" s="59" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AL29" s="59"/>
       <c r="AM29" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="AN29" s="62"/>
-      <c r="AO29" s="63">
+      <c r="AN29" s="72"/>
+      <c r="AO29" s="62">
         <v>0.01</v>
       </c>
       <c r="AQ29" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AR29" s="42" t="s">
-        <v>252</v>
+        <v>408</v>
       </c>
       <c r="AS29" s="1" t="s">
         <v>222</v>
       </c>
       <c r="AT29" s="42" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="AU29" s="1" t="s">
         <v>223</v>
@@ -8215,32 +8320,32 @@
       <c r="BH29" s="57"/>
       <c r="BI29" s="57"/>
       <c r="BJ29" s="57"/>
-      <c r="BL29" s="65">
+      <c r="BL29" s="63">
         <v>41233</v>
       </c>
-      <c r="BM29" s="66" t="s">
-        <v>343</v>
-      </c>
-      <c r="BN29" s="67">
+      <c r="BM29" s="64" t="s">
+        <v>341</v>
+      </c>
+      <c r="BN29" s="65">
         <v>32.42868</v>
       </c>
-      <c r="BO29" s="67">
+      <c r="BO29" s="65">
         <v>34.870280000000001</v>
       </c>
       <c r="BP29" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="BQ29" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="BR29" s="25"/>
       <c r="BW29">
         <v>6.5</v>
       </c>
-      <c r="BX29" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="BY29" s="71">
+      <c r="BX29" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY29" s="69">
         <v>4192.68</v>
       </c>
       <c r="BZ29"/>
@@ -8250,67 +8355,71 @@
       <c r="CD29"/>
       <c r="CE29"/>
       <c r="CF29"/>
+      <c r="CG29"/>
+      <c r="CH29"/>
     </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:86" x14ac:dyDescent="0.2">
+      <c r="AN30" s="73"/>
       <c r="AO30" s="13"/>
     </row>
-    <row r="31" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:86" x14ac:dyDescent="0.2">
+      <c r="AN31" s="73"/>
       <c r="AO31" s="13"/>
     </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:86" x14ac:dyDescent="0.2">
       <c r="AO32" s="13"/>
-      <c r="BM32" s="66"/>
+      <c r="BM32" s="64"/>
     </row>
     <row r="33" spans="41:70" x14ac:dyDescent="0.2">
       <c r="AO33" s="13"/>
-      <c r="BM33" s="66"/>
-      <c r="BQ33" s="67"/>
-      <c r="BR33" s="67"/>
+      <c r="BM33" s="64"/>
+      <c r="BQ33" s="65"/>
+      <c r="BR33" s="65"/>
     </row>
     <row r="34" spans="41:70" x14ac:dyDescent="0.2">
       <c r="AO34" s="13"/>
-      <c r="BM34" s="66"/>
-      <c r="BQ34" s="67"/>
-      <c r="BR34" s="67"/>
+      <c r="BM34" s="64"/>
+      <c r="BQ34" s="65"/>
+      <c r="BR34" s="65"/>
     </row>
     <row r="35" spans="41:70" x14ac:dyDescent="0.2">
       <c r="AO35" s="13"/>
-      <c r="BM35" s="66"/>
-      <c r="BQ35" s="67"/>
-      <c r="BR35" s="67"/>
+      <c r="BM35" s="64"/>
+      <c r="BQ35" s="65"/>
+      <c r="BR35" s="65"/>
     </row>
     <row r="36" spans="41:70" x14ac:dyDescent="0.2">
       <c r="AO36" s="13"/>
-      <c r="BM36" s="66"/>
-      <c r="BQ36" s="67"/>
-      <c r="BR36" s="67"/>
+      <c r="BM36" s="64"/>
+      <c r="BQ36" s="65"/>
+      <c r="BR36" s="65"/>
     </row>
     <row r="37" spans="41:70" x14ac:dyDescent="0.2">
       <c r="AO37" s="13"/>
-      <c r="BM37" s="66"/>
-      <c r="BQ37" s="67"/>
-      <c r="BR37" s="67"/>
+      <c r="BM37" s="64"/>
+      <c r="BQ37" s="65"/>
+      <c r="BR37" s="65"/>
     </row>
     <row r="38" spans="41:70" x14ac:dyDescent="0.2">
       <c r="AO38" s="13"/>
-      <c r="BM38" s="66"/>
-      <c r="BQ38" s="67"/>
-      <c r="BR38" s="67"/>
+      <c r="BM38" s="64"/>
+      <c r="BQ38" s="65"/>
+      <c r="BR38" s="65"/>
     </row>
     <row r="39" spans="41:70" x14ac:dyDescent="0.2">
       <c r="AO39" s="13"/>
-      <c r="BQ39" s="67"/>
-      <c r="BR39" s="67"/>
+      <c r="BQ39" s="65"/>
+      <c r="BR39" s="65"/>
     </row>
     <row r="40" spans="41:70" x14ac:dyDescent="0.2">
       <c r="AO40" s="13"/>
-      <c r="BQ40" s="67"/>
-      <c r="BR40" s="67"/>
+      <c r="BQ40" s="65"/>
+      <c r="BR40" s="65"/>
     </row>
     <row r="41" spans="41:70" x14ac:dyDescent="0.2">
       <c r="AO41" s="13"/>
-      <c r="BQ41" s="67"/>
-      <c r="BR41" s="67"/>
+      <c r="BQ41" s="65"/>
+      <c r="BR41" s="65"/>
     </row>
     <row r="42" spans="41:70" x14ac:dyDescent="0.2">
       <c r="AO42" s="13"/>

</xml_diff>

<commit_message>
Updating metadata for desalt bis bis
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/unige/desalt/metadata.xlsx
+++ b/metadata/excel/projects/unige/desalt/metadata.xlsx
@@ -16,10 +16,10 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -2661,10 +2661,10 @@
   </sheetPr>
   <dimension ref="A1:CD51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BQ1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="BZ41" sqref="BZ41"/>
+      <selection pane="bottomLeft" activeCell="CF34" sqref="CF34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2829,7 +2829,7 @@
       <c r="CB1" s="21"/>
       <c r="CC1" s="21"/>
     </row>
-    <row r="2" spans="1:82" s="53" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:82" s="53" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
         <v>46</v>
       </c>
@@ -8418,19 +8418,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -8448,14 +8438,24 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>